<commit_message>
topic modeling dan indobart
</commit_message>
<xml_diff>
--- a/benc_result/01-indobart-bertopic/topic_info.xlsx
+++ b/benc_result/01-indobart-bertopic/topic_info.xlsx
@@ -468,7 +468,7 @@
         <v>-1</v>
       </c>
       <c r="C2" t="n">
-        <v>4668</v>
+        <v>4714</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -477,12 +477,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>['indonesia', 'jakarta', 'orang', 'negara', 'kpk', 'anak', 'rp', 'salah', 'memiliki', 'presiden']</t>
+          <t>['indonesia', 'jakarta', 'orang', 'negara', 'anak', 'salah', 'kota', 'kpk', 'presiden', 'rp']</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>['Suara.com - Sepuluh orang tewas dalam unjuk rasa di Iran pada Minggu, kata televisi setempat pada Senin (1 / 1 / 2018). Unjuk rasa puluhan ribu orang di berbagai kota tersebut menunjukkan perlawanan terbesar warga terhadap kepemimpinan Iran sejak kerusuhan pro - reformasi pada 2009. Selain itu, seruan untuk meneruskan gerakan tersebut memunculkan kekhawatiran akan keguncangan politik. Baca_Juga " Dalam beberapa kejadian tadi malam, sekitar 10 orang tewas di beberapa kota, " kata stasiun televisi pemerintah tanpa menjelaskan lebih lanjut. Iran adalah salah satu negara penghasil terbesar minyak dunia dan kekuatan utama kawasan, yang terlibat dalam kemelut kawasan di Suriah dan Yaman untuk memperebutkan pengaruh dengan Arab Saudi. Keterlibatan Iran dalam sengketa kawasan itu membuat warga kecewa karena mereka ingin pemerintah lebih fokus menciptakan lapangan kerja daripada menghabiskan uang negara untuk perang di luar negeri. Unjuk rasa pertama kali muncul di kota terbesar kedua Iran, Masshad, untuk menentang kenaikan harga-harga. Unjuk rasa itu kemudian meluas ke berbagai kota lain dan berkembang menjadi demonstrasi politik anti - pemerintah. Sejumlah pengunjuk rasa bahkan meminta pemimpin agung Ayatollah Ali Khamenei untuk mundur dan menuding pemerintah sebagai pencuri. Mereka mengaku marah atas korupsi dan krisis ekonomi di negara yang tingkat pengangguran anak mudanya mencapai 28,8 persen pada tahun lalu. Unjuk rasa terus berlangsung sampai Minggu (31 / 12 / 2017) malam meskipun Presiden Hassan Rouhani meminta warga untuk kembali tenang. Dalam pidatonya, Rouhani mengatakan bahwa warga Iran memang berhak untuk mengkritik pemerintah, namun juga memperingatkan akan adanya pembubaran. " Pemerintah tidak akan membiarkan mereka yang merusak fasilitas umum, melanggar aturan, dan menciptakan kerusuhan, " kata Rouhani. Hingga kini ratusan orang telah ditangkap. Dua orang tewas ditembak di kota Izeh pada Minggu dan sejumlah orang lain terluka, demikian berita dari ILNA. Hingga kini belum diketahui apakah dua orang itu termasuk bagian dari 10 orang tewas yang diberitakan stasiun televisi negara. " Saya tidak tahu apakah penembakan itu dilakukan oleh pengunjuk rasa atau polisi. Kasus ini tengah diselidiki, " kata anggota parlemen Hedayatollah Khademi sebagaimana dikutip ILNA. Sementara itu, di kota Shahin Shahr, demonstrasi berujung pada kerusuhan. Sejumlah video menunjukkan para pengunjuk rasa menyerang polisi dan menghancurkan sebuah mobil. Untuk menanggapi unjuk rasa di berbagai kota itu, pemerintah menyatakan akan membatasi akses terhadap aplikasi pengirim pesan Telegram dan Instagram. Selain itu, muncul sejumlah laporan tentang kehilangan akses Internet di sejumlah wilayah. (Antara)', 'Jakarta (ANTARA News) - Komisi Pemberantasan Korupsi (KPK) memeriksa mantan Ketua DPR RI 2009 - 2014 Marzuki Alie dalam penyidikan tindak pidana korupsi pengadaan paket penerapan Kartu Tanda Penduduk berbasis Nomor Induk Kependudukan secara nasional (KTP - e). " Yang bersangkutan diperiksa sebagai saksi untuk tersangka Anang Sugiana Sudihardjo, " kata Juru Bicara KPK Febri Diansyah di Jakarta, Senin. Marzuki tampak sudah mendatangi gedung KPK sekitar pukul 10.05 WIB, namun ia tak banyak berkomentar soal pemanggilannya kali ini. " Nanti saja ya, " kata dia singkat. Nama Marzuki pernah disebut dalam dakwaan perkara KTP - e dengan terdakwa mantan Direktur Jenderal Kependudukan dan Pencatatan Sipil Kementerian Dalam Negeri Irman dan mantan Direktur Pengelolaan Informasi Administrasi Kependudukan Kementerian Dalam Negeri Sugiharto. Marzuki disebut menerima Rp 20 miliar terkait proyek KTP - e sebesar Rp 5,95 triliun itu. Selain memeriksa Marzukie, KPK juga dijadwalkan akan memeriksa dua mantan Ketua Kelompok Fraksi (Kapoksi) di Komisi II DPR RI masing-masing Abdul Malik Haramain dari Fraksi Partai Kebangkitan Bangsa (PKB) dan Djamal Aziz dari Fraksi Partai Hanura. Dalam dakwaan Irman dan Sugiharto, keduanya selaku Ketua Kelompok Fraksi (Kapoksi) di Komisi II DPR RI juga disebut menerima masing-masing 37 ribu dolar AS. Anang Sugiana Sudihardjo merupakan Direktur Utama PT Quadra Solution yang ditetapkan sebagai tersangka kasus KTP - e pada 27 September 2017. PT Quadra Solution merupakan salah satu perusahaan yang tergabung dalam konsorsium Percetakan Negara Republik Indonesia (PNRI) sebagai pelaksana proyek KTP - elektronik (KTP - e) yang terdiri dari Perum PNRI, PT LEN Industri, PT Quadra Solution, PT Sucofindo, dan PT Sandipala Artha Putra. Anang Sugiana Sudihardjo diduga dengan tujuan menguntungkan diri sendiri atau orang lain atau suatu korporasi menyalahgunakan kewenangan, kesempatan atau sarana yang ada padanya karena kedudukannya atau jabatannya sehingga diduga mengakibatkan kerugian negara sekurang-kurangnya Rp 2,3 triliun dari nilai paket pengadaan sekitar Rp 5,9 triliun dalam paket pengadaan KTP - e pada Kemendagri. Indikasi peran Anang Sugiana Sudihardjo terkait kasus itu antara lain diduga dilakukan bersama-sama dengan Setya Novanto, Andi Agustinus alias Andi Narogong, Irman dan Sugiharto dan kawan-kawan. Anang Sugiana Sudihardjo diduga berperan dalam penyerahan uang terhadap Setya Novanto dan sejumlah anggota DPR RI melalui Andi Agustinus alias Andi Narogong terkait dengan proyek KTP - e. Anang Sugiana Sudihardjo disangka melanggar pasal 2 ayat (1) atas pasal 3 UU No 31 Tahun 1999 sebagaimana telah diubah dengan UU No 20 Tahun 2001 tentang Pemberantasan Korupsi jo pasal 55 ayat (1) ke - 1 KUHP.', 'Jakarta (ANTARA News) - Pemerintah Provinsi DKI Jakarta hari ini meluncurkan sistem pemantauan terintegrasi Jakarta Satu, yang memadukan semua data di pemerintah provinsi. " Program ini akan mengintegrasikan semua data yang ada di jajaran Pemprov DKI. Jakarta Satu maksudnya adalah Satu Peta, Satu Data dan Satu Kebijakan, " kata Gubernur DKI Jakarta Anies Baswedan di Balai Kota, Jakarta Pusat, Rabu. Pemerintah Provinsi DKI Jakarta bekerja sama dengan Komisi Pemberantasan Korupsi (KPK) dalam menerapkan sistem itu. Pada tahap pertama, Anies menjelaskan, Sistem Jakarta Satu akan diterapkan di Kecamatan Gambir dengan melibatkan empat Satuan Kerja Perangkat Daerah (SKPD) yakni Dinas Cipta Karya Tata Ruang dan Pertanahan (CKTRP), Dinas Kependudukan dan Pencatatan Sipil, Badan Pajak dan Retribusi Daerah (BKRD) serta Dinas Perindustrian dan Energi (DPE) DKI Jakarta. " Jadi, nanti data dasar akan disusun oleh Dinas CKTRP. Kemudian diintegrasikan dengan data kependudukan, pajak dan retribusi, serta data air. Ini baru fase awal, " ujar Anies. Dia menuturkan bahwa dengan sistem Jakarta Satu, kebijakan Pemerintah Provinsi DKI dapat dilakukan secara konsisten karena berdasarkan pada kesamaan data dan informasi. Wakil Ketua KPK Saut Situmorang menyambut baik kerja sama dengan Pemprov DKI Jakarta dalam sistem Jakarta Satu. Selain melakukan penindakan, KPK juga memiliki tugas dalam pencegahan korupsi. " Melalui sistem Jakarta Satu, kami berharap tindak korupsi di jajaran pemerintah daerah dapat dicegah secara efektif. Kami juga berharap sistem ini dapat menjadi model pencegahan korupsi di daerah lainnya, " kata Saut.']</t>
+          <t>['Merdeka.com - Wakil Ketua Pansus Angket KPK Masinton Pasaribu mengatakan pemanggilan Presiden Jokowi bisa saja dilakukan untuk menanyakan respons soal 4 temuan penyimpangan kinerja KPK. Pemanggilan presiden, kata Masinton, telah diatur dalam UU. " Ya bisa saja pemanggilan terhadap siapa pun. UU memperkenankan memanggil siapa pun dalam panitia angket ini, " kata Masinton di Komplek Parlemen, Senayan,   Jakarta, Rabu (23 / 8). Menurutnya, Presiden Jokowi bisa mendelegasikan ke pihak lain untuk datang ke rapat Pansus jika tengah sibuk menjalankan tugas. Namun hingga saat ini, Pansus belum merencanakan untuk memanggil Presiden. " Belum, belum kita belum memutuskan. Tapi ide itu wajar-wajar saja, " tukasnya. Nantinya, pertemuan Pansus angket KPK dan Presiden akan dilakukan dalam bentuk rapat konsultasi. Akan tetapi, dimungkinkan juga DPR yang datang ke Istana bertemu dengan Presiden. Yang terpenting, kata Masinton, terdapat kesepahaman antara DPR dan Presiden untuk membenahi lembaga KPK. " Bisa aja dalam bentuk forum konsultasi antara pemimpin negara rapat antara lembaga negara, " jelas dia. Secara pribadi, Masinton menilai langkah perbaikan lembaga KPK diperlukan lantaran upaya pemberantasan   korupsi yang dijalankan KPK cenderung stagnan. " Kita sudah 15 tahun pemberantasan korupsi kita, tapi kita stagnan, ya gini gini aja, " pungkasnya. Sebelumnya, Wakil Ketua Dewan Perwakilan Rakyat (DPR) Fahri Hamzah mengusulkan agar pemerintah terutama Presiden Joko Widodo dan Wakil Presiden Jusuf Kalla turun tangan menindaklanjuti 4 temuan Pansus angket KPK indikasi penyimpangan kinerja KPK. 4 temuan penyimpangan kinerja KPK itu yakni menyangkut tata kelola kelembagaan, sistem penegakan hukum, masalah SDM, dan tata kelola anggaran KPK. " Pak Jokowi dan JK sebagai pimpinan kabinet harus mulai mengondisikan, apapun temuan DPR ini harus dipandang secara positif dan harus ada follow up secara positif juga dari pihak pemerintah, " ujar Fahri. Bahkan, Fahri mengusulkan agar Pansus memanggil Presiden Jokowi untuk diminta keterangan soal koordinasi KPK. Sebab, selama ini KPK dinilai bekerja tanpa koordinasi dengan Presiden. " Saya misalnya mengusulkan agar presiden harusnya ditanya. Bagaimana sebetulnya ada KPK yang bekerja tanpa koordinasi dengan presiden. Saya sendiri seharusnya presiden dihadirkan. Bagaimana tanggapan presiden, " ujarnya. " Apakah memang menurut presiden wajar ada lembaga yang bekerja, satu sisi presidennya ngomong ke mana mana kita anti korupsi tapi orang ditangkap ada setiap hari. Apa enggak ganjil di kepala presiden? Trus fungsi presiden dalam memberantas korupsi apa? Wong tiap hari ada korupsi kok, " sambungnya. [bal]', 'Rimanews - Koordinator Divisi Hukum dan Monitoring Peradilan Indonesia Corruption Watch (ICW) Emerson Yuntho menyarankan Komisi Pemberantasan Korupsi (KPK) perlu membentuk unit keamanan khusus supaya tak \xa0 ketergantungan kepada aparat kepolisian. " Belajar dari kejadian upaya teror terhadap KPK selama hampir 14 tahun terakhir, maka sudah seharusnya KPK punya unit keamanan tersendiri, " kata Emerson melalui keterangan tertulisnya di Jakarta, Jumat (14 / 04 / 201 " Unit ini mengadopsi seperti tim " Special Weapons and Tactics " (SWAT) di Kepolisian Amerika Serikat. Mereka direkrut dan dilatih secara khusus dan bahkan dapat dipersenjatai, " lanjutnya. Ia menjelaskan unit keamanan KPK itu bertugas antara lain sebagai pengawal penyidik, pegawai dan pimpinan KPK dalam kondisi khusus, melakukan operasi senyap atau pengamanan untuk membantu tugas - tugas di bidang penindakan termasuk operasi tangkap tangan, dan melakukan pengusutan dan penangkapan pelaku teror terhadap KPK. " Anggota tim direkrut secara mandiri oleh KPK sehingga memiliki loyalitas terhadap KPK, bukan ke instansi lain, " ucap Emerson. Sebelumnya, salah satu penyidik KPK Novel Baswedan disiram air keras sepulang shalat subuh pada Selasa (11 / 4). Juru Bicara KPK Febri Diansyah mengatakan Novel masih menjalani proses pengobatan di salah satu rumah sakit di Singapura. " Sejak kedatangan kemarin (Rabu, 12 / 4) langsung dilakukan beberapa diaognasa dan tindakan - tindakan cepat, baik untuk mata maupun untuk bagian kulit lain di wajah yang terkena air keras tersebut. Setelah dilakukan diagonasa dan perawatan untuk kulit yang terkena air keras atau luka bakar tersebut sudah mulai ada perbaikan dan untuk mata masih membutuhkan perawatan lebih intensif, " kata Febri di gedung KPK, Jakarta, Kamis (13 / 4). Ia menyatakan biaya perawatan Novel Baswedan akan ditanggung menggunakan anggaran pendapatan dan belanja negara (APBN). " Biaya perawatan tetap dari APBN dan proses - prosesnya tetap tentu saja menggunakan mekanisme keuangan negara, " kata Febri. Novel adalah salah satu penyidik senior KPK yang antara lain menangani kasus korupsi dalam pengadaan Kartu Tanda Penduduk Elektronik (KTP - E).', 'JAKARTA (Pos Kota) – Kuasa hukum Basuki Tjahaja Purnama (Ahok), I Wayan Sudirta, mengatakan belum mendapatakan pemberitahuan terkait rencana Komisi Pemberantasan Korupsi (KPK) yang akan memanggil kliennya untuk dimintai keterangan dalam kasus suap reklamasi. Wayan mengatakan sebagai kuasa hukum belum mengetahui rencana pemanggilan Ahok itu. “ Belum mendengar. Belum cerita belum dengar saya juga belum tahu apakah ada surat itu atau belum, ” katanya saat dihubungi, Senin (6 / 11 / 2017). Wayan mengatakan telah mendapatkan pemanggilan resmi dari KPK, hal itu akan didiskusikan dengan Ahok. Namun Wayan memastikan mantan Gubernur DKI Jakarta itu akan memenuhi proses hukum yang berjalan. “ Pak Ahok kan orang taat hukum, nanti kalau ada pemanggilan kita rundingkan. Pada prinsipnya kan Pak Ahok ini orang taat hukum. Sangat menghargai proses, prosedur hukum, ” tandas Wayan. Saat ini Ahok tengah menjalani masa hukuman penjara di Rutan Mako Brimob, Kelapa Dua, Depok, Jawa Barat. Ahok dinyatakan bersalah oleh Pengadilan Negeri Jakarta Utara melakukan tindak pidana penistaan agama. Dalam kasus tersebut Ahok dihukum dua tahun penjara. Sebelumnya, KPK mengisyaratkan memeriksan mantan Gubernur Ahok dan Djarot Saiful Hidayat. Ini dilakukan menyusul menguatnya dugaan praktek suap di proyek reklamasi Teluk Jakarta, Dugaan tersebut terkait pembahasan Rancangan Peraturan Daerah (Raperda) tentang Rencana Tata Ruang Kawasan Strategis Pantai Utara Jakarta (RTRKSP) atau Raperda Reklamasi. “ Kalau penyidik atau penyelidik kami menganggap itu penting, maka siapapun yang dianggap mengetahui akan dipanggil untuk dimintai keterangan, ” tegas Wakil Ketua KPK Laode Muhammad Syarif, Minggu (5 / 11 / 2017). Adapun penyelidikan KPK terhadap adanya dugaan suap izin reklamasi Teluk Jakarta baru diketahui setelah pada Jumat (27 / 10) memanggil Sekretaris Daerah DKI Jakarta, Saefullah. Kali ini, lembaga antirasuah tengah mendalami keterlibatan korporasi di kasus suap pembahasan Raperda Reklamasi tersebut. (ikbal / yp)']</t>
         </is>
       </c>
     </row>
@@ -494,21 +494,21 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>3344</v>
+        <v>3161</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0_pemain_gol_laga_musim</t>
+          <t>0_pemain_gol_musim_laga</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>['pemain', 'gol', 'laga', 'musim', 'menit', 'tim', 'liga', 'pertandingan', 'bola', 'madrid']</t>
+          <t>['pemain', 'gol', 'musim', 'laga', 'menit', 'tim', 'liga', 'pertandingan', 'madrid', 'bola']</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>['Barcelona sukses meraih kemenangan ketiganya secara beruntun di awal bergulirnya La Liga Spanyol musim ini, setelah menaklukkan Espanyol lewat skor telak 5 - 0 dalam laga derby Catalan, Minggu (10 / 9) dini hari WIB. Lionel Messi kembali menunjukkan ketajamannya melalui hat-trick yang berhasil ia catatkan di laga yang berlangsung di Camp Nou ini. Sementara dua gol lainnya dicetak oleh Gerard Pique dan Luis Suarez di penghujung pertandingan. Tim asuhan Ernesto Valverde tersebut berhasil membuka keunggulan saat laga memasuki menit ke - 26. Menerima umpan terobosan Ivan Rakitic, Messi mampu menembus pertahanan Espanyol dan melepaskan tendangan keras di kotak penalti yang tak dapat dihalau kiper lawan Pau Lopez. Gol tersebut membuat Messi tercatat sebagai top scorer sepanjang di laga derby Catalan dalam ajang La Liga. Empat menit berselang giliran Rakitic yang mengancam gawang Espanyol setelah melakukan kerja sama satu-dua dengan Messi. Namun tendangan gelandang asal Kroasia itu dari jarak dekat masih bisa dihalau secara brilian oleh penjaga gawang berusia 22 tahun milik Espanyol. SIMAK JUGA: \xa0 Sevilla Raih Poin Penuh Atas Eibar Barca kemudian sukses menggandakan keunggulan pada menit ke - 35. Messi kembali berhasil mencetak gol. Melalui serangan balik cepat, bola yang Messi kuasai sebenarnya sempat memantul mengenai bek lawan, namun bola liar mengarah ke Jordi Alba yang kemudian memberikan umpan mendatar kepada bintang asal Argentina itu di muka gawang. SIMAK JUGA: \xa0 Kemenangan Belum Mau Hampiri Madrid Espanyol bukannya tanpa perlawanan di laga ini. Mereka nyaris mencetak gol pada menit ke - 41. Pablo Piatti melepaskan tendangan keras namun bola masih mengenai tiang gawang Barca yang dikawal Marc - Andre ter Stegen. Pesta gol Barca kemudian baru berlanjut di babak kedua. Messi berhasil mencatatkan gol ketiganya di laga ini. Penyerang berusia 30 tahun itu kembali sukses memaksimalkan umpan silang Jordi Alba dari sisi kiri kotak penalti Espanyol. Alba sukses mencatatkan dua assist di laga ini. Itu menjadi yang kedua kalinya sang bek kiri berhasil memberikan kontribusi seperti itu, sebelumnya ia pernah melakukannya di laga kontra Osasuna pada Desember 2016. Memasuki menit-menit akhir laga, Espanyol nampak sudah menyerah. Barca pun sukses menambah golnya pada menit ke - 87. Memanfaatkan sepak pojok Rakitic, Pique mampu menyundul bola dan menciptakan gol keempat untuk timnya di laga ini. Gol tersebut kemudian disusul oleh aksi Luis Suarez yang sukses mencatatkan namanya di papan skor setelah menerima umpan silang sang pemain baru Ousmane Dembele pada menit ke - 90.', 'Lengkap sudah pencapaian Manchester United di kancah Eropa. Kini, The Red Devils menjadi tim yang telah memenangi seluruh trofi dari berbagai turnamen Benua Biru. Liga Champions, Piala Winners, Piala Super Eropa, dan terakhir...Liga Europa. Dari sekian banyak trofi yang diraih, baru tahun ini Liga Europa berada dalam genggaman. Tak peduli dengan stigma yang melekat sebagai turnamen kasta kedua, United   tetap menikmati setiap perjalanan hingga menuju tangga juara. Apalagi, kesuksesan merengkuh trofi Liga Europa memberikan keuntungan ganda yakni lolos ke Liga Champions musim depan. Sejak jauh-jauh hari, juru latih United Jose Mourinho menegaskan bakal mempersiapkan timnya secara total guna memenangi partai final melawan Ajax Amsterdam di Friends Arena, Solna, Swedia, Kamis (25 / 5 / 2017) dini hari WIB. Kebijakan merotasi besar-besaran pemain pun diberlakukan kala United melakoni partai pamungkas Premier League pada akhir pekan lalu. Terbukti, kebijakan pragmatis Mou itu membuahkan hasil manis dengan kemenangan dua gol tanpa balas. " Ini akhir dari musim yang sulit. Mungkin musim tersulit saya sebagai pelatih. Tapi, saya pikir kami menjalani musim yang bagus. Kami lebih memilih cara ini (menuju Liga Champions) daripada finis di posisi empat, tiga, atau dua klasemen. Kami mencapai objektif kami yaitu Liga Champions. Tim ini sekarang merupakan tim yang meraih setiap gelar juara di sepak bola dunia, " ujar Mou sesuai laga puncak seperti dilansir ESPN. " Kami sangat senang karena berjuang keras untuk mendapatkan (trofi) ini. Sejak awal, kami menanamkan hal ini dalam pikiran kami. Kami selalu berpikir bisa memenangi Liga Europa. Dan, kami sangat bahagia, terutama karena cara kami bermain di final, " sambungnya. Seperti biasa, Mou dengan kepercayaan diri selangitnya, menilai skuat asuhannya tampil lebih superior dari sang lawan. " Kami tahu bagaimana meraih kemenangan. Dan, meraihnya dengan cara yang nyaman. Mereka tim yang bagus, tapi kami jauh lebih kuat, " tegasnya. Mantan arsitek Chelsea ini kemudian membocorkan rahasia kemenangan timnya. Skema main yang diusung Marcus Rashford dan kawan-kawan menjadi kunci untuk meredam permainan Ajax yang dominan dalam penguasaan bola. " Jika Anda ingin melakukan pressing terus-menerus, jangan main bola-bola pendek. Jika Anda dominan di area tertentu, maka mainlah bola-bola panjang. Kami tahu di mana mereka lebih baik daripada kami dan kami tahu di mana kekuatan kami, " ucapnya. Sepanjang 90 menit, United tampak membiarkan Ajax berlama-lama menguasai bola. Tercatat, wakil Belanda memiliki ball possesion hingga 69:31. Namun, United mengantisipasinya dengan menerapkan pertahanan yang sangat dalam. Terbukti, para pemain Ajax terlihat kesulitan menembusnya. Gawang Sergio Romero pun hanya terancam sebanyak tiga kali dari 17 kali percobaan yang dilepaskan Hakim Ziyech dan kawan-kawan. Sebaliknya, Mou memilih mengeksploitasi kekuatan fisik dari para pemainnya seperti Chris Smalling, Marouane Fellaini, dan Paul Pogba. Berulang kali, ketiga pemain itu memenangi duel bola atas dan juga area. Efektivitas permainan United pun berjalan cukup lancar dengan mencatatkan empat tembakan tepat sasaran dari tujuh kali percobaan dan dua di antaranya berbuah gol. " Kami mencoba membunuh kualitas bagus mereka dan mengeksploitasi kelemahan mereka. Dan, kami melakukannya dengan sangat baik sejak menit pertama. Kami benar-benar pantas meraih trofi ini, " tegas Mou. Raihan trofi Liga Europa kali ini juga bermakna terasa sangat mendalam bagi Mou dan pasukannya. Itu tak lepas dari aksi bom bunuh diri di Manchester Arena yang terjadi hanya dua hari menjelang partai final. Pelatih yang meraih treble bersama Inter Milan ini berharap torehan gelar juara bisa memberikan sedikit senyuman kepada warga Manchester. " Ini sungguh berat dan Anda juga tahu kami tak melakukan konferensi pers pada Selasa lalu. Saya setuju dengan keputusan UEFA untuk tetap melangsungkan pertandingan dan   berharap kemenangan ini bisa memberikan kebahagian. Jika kami bisa mengubah hidup orang dari trofi ini, kami tak akan berpikir dua kali. Apakah piala ini membuat Kota Manchester sedikit berbahagia? Mungkin, " katanya. " Tapi, yang pasti kami datang ke sini untuk melakukan pekerjaan kami. Kami tak bisa menyembunyikan kebahagian kami karena ketika Anda menang maka Anda otomatis akan senang dan bangga. Para pemain fantastis. Mereka membuang semua hal non - teknis dan berkonsentrasi penuh kepada pertandingan, " pungkasnya.', 'Paul Pogba yang telah pulih dari cedera langsung memberikan kontribusi besar lewat satu gol dan assist saat membantu Manchester United membalikkan kedudukan dan berhasil menang telak 4 - 1 saat menjamu Newcastle United di ajang Liga Primer Inggris, Sabtu (18 / 11). Berlaga di Old Trafford, suporter tuan rumah sempat terdiam setelah Newcastle mampu mencetak gol lebih dulu saat laga memasuki menit ke - 14 lewat gol Dwight Gayle. Bek Manchester United Victor Lindelof gagal mengantisipasi umpan silang DeAndre Yedlin, dan bola pun kemudian disambut oleh tendangan Gayle yang sukses berbuah gol setelah memperdaya sang kiper David De Gea. Gol tersebut membuat Manchester United kebobolan dari permainan terbuka di Old Trafford untuk pertama kalinya dalam ajang Liga Primer sejak laga di tahun baru 2016 atau tepatnya setelah 21 jam 37 menit. Manchester United hampir saja tertinggal lebih jauh, namun beruntung Jacob Murphy gagal memaksimalkan peluangnya. Tuan rumah justru mampu bangkit lewat dua gol sebelum babak pertama berakhir. Gol penyeimbang bagi tim asuhan Jose Mourinho tercipta lewat sundulan Anthony Martial pada menit ke - 37. Ia berhasil memaksimalkan umpan silang kompatriotnya asal Prancis, Pogba, dari sisi kanan kotak penalti Newcastle. Memasuki injury time babak pertama United mampu membalikkan kedudukan. Lagi - lagi mereka sukses mencetak gol lewat sundulan. Kali ini Chris Smalling yang mampu menjebol gawang Newcastle setelah memanfaatkan umpan lambung Ashley Young dari sisi kiri. Di babak kedua United berhasil menambah keunggulannya lewat gol Pogba dan sang penyerang Romelu Lukaku. Pogba berhasil mencetak gol setelah menuntaskan umpan sundulan Marcus Rashford di mulut gawang pada menit ke - 54. Sementara gol keempat tuan rumah tercipta pada menit ke - 70 lewat tendangan keras Lukaku di kotak penalti setelah melakukan kerja sama satu-dua dengan Juan Mata. Selain mampu unggul tiga gol, suporter di Old Trafford juga nampak senang saat Zlatan Ibrahimovic, yang telah pulih dari cedera lutut, masuk menggantikan Martial pada menit ke - 77. Setiap sentuhan yang dilakukan Ibrahimovic selalu mendapatkan pujian dari para suporter. Penyerang berkebangsaan Swedia itu juga nyaris saja menciptakan gol, namun tendangan volinya masih bisa dihalau kiper Newcastle Rob Elliot. Tapi setidaknya itu telah memperlihatkan kemampian pemain berusia 36 tahun itu tidak berkurang setelah absen panjang sejak April lalu. Kemenangan tersebut membuat United terus menjaga jarak dengan pemuncak klasemen Manchester City. The Red Devils kini tetap menempati urutan kedua dengan perolehan 26 poin, tertinggal delapan poin dari rival sekotanya.']</t>
+          <t>['Dua gol dari Isco berkontribusi membawa Spanyol sukses mengungguli Italia 3 - 0 dalam lanjutan laga kualifikasi Piala Dunia 2018, Minggu (3 / 9) dini hari WIB. Tim asuhan Julen Lopetegui itu menampilkan starting XI tanpa penyerang murni. Ia memainkan Isco sebagai false nine, dan keputusan tersebut nampaknya sukses membuat pertahanan Italia goyah. Bintang muda Real Madrid Marco Asensio juga dipercaya menjadi starter di laga ini. Dalam laga yang berlangsung di Santiago Bernabeu tersebut \xa0 Spanyol mampu terus menguasai bola, sementara Italia yang berjuang keras merebutnya justru kerap melakukan pelanggaran. Pada menit ke - 4 Marco Verratti telah mendapatkan kartu kuning dari wasit asal Belanda Bjorn Kuipers. SIMAK JUGA - REVIEW: Denmark Hancurkan Polandia Spanyol pun bisa memecah kebuntuan setelah bek Italia Leonardo Bonucci mendapatkan kartu kuning karena melakukan tekel keras di area dekat kotak penalti. Melalui tendangan bebas yang sukses dieksekusi dengan sempurna oleh Isco pada menit ke - 13, tim tuan rumah mampu unggul. Tendangan keras gelandang Real Madrid itu mampu melewati pagar betis dan tak dapat dijangkau oleh sang kiper veteran Italia Gianluigi Buffon. Itu merupakan gol tendangan bebas yang pertama dari Isco untuk timnas Spanyol. Ia menciptakannya dalam percobaan kedua. Tertinggal satu gol Italia mulai membalas serangan. Pada menit ke - 22 Andrea Belotti menyundul umpan silang dari Matteo Darmian, namun bola masih bisa diselamatkan dengan cemerlang oleh kiper Spanyol David de Gea. SIMAK JUGA: \xa0 Perkuat Timnas Spanyol U - 21, Gelandang Real Madrid Alami Cedera Leher Memasuki menit ke - 40 Spanyol berhasil menggandakan keunggulannya. Isco kembali berhasil membobol gawang Buffon. Ia menerima operan dari Andres Iniesta sebelum melepaskan tendangan mendatar dari area luar kotak penalti Italia. Hingga 45 menit pertama berakhir tidak ada lagi gol yang tercipta. Terakhir kali Italia mengakhiri babak pertama dengan ketertinggalan dua gol terjadi pada final 2012, kala itu mereka menghadapi lawan yang sama, Spanyol. Saat para pemain menuju ruang ganti usai babak pertama berakhir nama Isco pun terus diteriakkan oleh para suporter yang hadir di Santiago Bernabeu. Di babak kedua situasi tidak banyak berubah. Spanyol masih berupaya untuk terus menguasai bola. Italia yang ingin mengejar ketertinggalan tidak tinggal diam, tim asuhan Giampiero Ventura itu \xa0 beberapa kali mencoba melakukan serangan namun tak kunjung membuahkan hasil. SIMAK JUGA - \xa0 Alvaro Morata: Gianluigi Buffon Adalah Alien &amp; Kiper Terbaik Sepanjang Masa Akan tetapi Spanyol justru mampu melakukan serangan balik dan menciptakan gol ketiganya di laga ini pada menit ke - 77. Sergio Ramos yang berlari ke arah pertahanan Italia melepaskan umpan silang yang kemudian berhasil dituntaskan oleh Alvaro Morata di mulut gawang. Kemenangan ini membuat Spanyol unggul tiga poin dari Italia di grup G dengan tiga laga lagi yang tersisa. Spanyol juga berhasil memperpanjang catatan tak terkalahkannya di ajang kualifikasi Piala Dunia menjadi 60 laga. Mereka mampu 47 kali menang dan imbang 13 kali. Sementara bagi Italia ini merupakan kekalahan pertama di ajang kualifikasi Piala Dunia \xa0 setelah melewati 33 laga. Sebelumnya mereka mampu menang 23 kali dan sisanya berakhir imbang. Di laga berikutnya Spanyol akan menghadapi juru kunci grup Liechtenstein, sementara Italia akan menjamu Israel pada Rabu (6 / 9) dini hari WIB.', "Manchester United meraih kemenangan penting seiring keberhasilan mereka mengatasi perlawanan Everton dengan skor 4 - 0 dalam lanjutan Liga Primer Inggris matchday kelima, Minggu (17 / 9) malam WIB. Bermain di depan pendukungnya sendiri di Old Trafford, United yang tampil tanpa Paul Pogba langsung tampil menekan begitu babak pertama digulirkan. Gol cepat bahkan berhasil mereka ciptakan di menit keempat setelah Antonio Valencia menyambar bola hasil kiriman umpan Nemanja Matic, yang sekaligus menaklukkan kiper Jordan Pickford. Everton yang tertinggal terus berada dalam tekanan tim tuan rumah. Akan tetapi mereka baru berani keluar menyerang saat memasuki pertengahan laga, dengan klub asal Liverpool itu melancarkan serangan balik cepat yang nyaris dikonversi menjadi gol oleh Wayne Rooney. Kesempatan emas tersebut dimiliki eks kapten Setan Merah ini di menit ke - 21, namun sayang tendangannya memanfaatkan umpan silang Cuco Martina masih melebar dari gawang. United sendiri tidak panik. Mereka mencoba kembali mengontrol permainan dan nyaris memperbesar kedudukan memasuki setengah jam. Meski demikian, harapan tersebut tidak terlaksana lantaran Romelu Lukaku yang tinggal berhadapan dengan kiper lawan justru gagal memanfaatkan kecerobohan Michael Keane dan tendangannya tidak tepat ke sasaran. Di laga ini, Everton arahan Ronald Koeman sempat mengoyak jala gawang David de Gea saat babak pertama berlangsung, tapi gol tersebut dianulir mengingat gelandang Tom Davies telah terlebih dahulu terjebak dalam posisi offside dan setelahnya tidak banyak peluang yang tercipta hingga wasit memerintahkan kedua kubu untuk masuk ruang ganti. SIMAK JUGA: Alvaro Morata Benarkan Ketertarikan Manchester United Di Musim Panas Memasuki babak kedua, baik United dan Everton tetap mempertahankan formasi seperti babak pertama. Di babak ini tamu memiliki peluang untuk menyamakan skor tak lama setelah restart, namun tendangan Rooney dari jarak dekat masih bisa diblok oleh De Gea yang menunjukkan refleks luar biasa. Everton tampil lebih baik di paruh kedua ini. Mereka bahkan mampu memberi perlawanan untuk United dan beberapa kali terlihat nyaris mencetak gol. Yang kurang dari mereka adalah ketenangan di depan gawang dan itu sejalan dengan sejumlah kesempatan yang mereka buang. Terlihat kehilangan kontrol permainan, manajer Jose Mourinho lantas memilih untuk menarik keluar Marcus Rashford, yang di pertandingan ini tidak memiliki sentuhan terbaik. Posisinya kemudian digantikan oleh Jesse Lingard di satu jam permainan guna memberi sedikit keseimbangan di lini tengah. Masuknya Lingard secara perlahan membuat United kembali ke penguasaan dan mereka hampir mencetak gol kedua andai tendangan bebas Juan Mata tidak membentur mistar. Sebaliknya, Everton memutuskan untuk menarik keluar Rooney di menit ke - 82, dan itu menjadi awal dari akhir perlawanan klub asal Liverpool tersebut. Pasukan Mourinho baru benar-benar mengemas gol keduanya lewat lesakan Henrikh Mkhitaryan di menit ke - 83 memanfaatkan sodoran umpan Lukaku. Dan penyerang Belgia Lukaku memperbesar keunggulan timnya enam menit berselang lewat sebuah sontekan yang tidak mampu diantisipasi Pickford, yang di akhir pertandingan gawangnya terpaksa bobol kembali berkat penalti pemain pengganti Anthony Martial. Adapun kemenangan ini seolah menjadi penegasan United akan statusnya sebagai calon juara, dengan mereka untuk sementara menempel ketat Manchester City di puncak klasemen. Sementara itu, kekalahan ini membuat Everton terpuruk di posisi ke - 18 setelah baru merangkum empat poin dari lima laga perdana. Susunan Pemain Manchester United: De Gea; Valencia, Bailly, Jones, Valencia; Fellaini, Matic; Mata (Herrera 77'), Mkhitaryan (Martial 88'), Rashford (Lingard 61’); Lukaku. Everton: Pickford; Keane, Williams, Jagielka; Martina, Gueye (Calvert - Lewin 76'), Schneiderlin, Baines; Davies (Sandro 66'), Sigurdsson; Rooney (Mirallas 82').", 'INGGRIS - Bagi Jose Mourinho Piala FA sangatlah penting. Sebab bisa jadi gelar ini yang mamu diraih Manchester United musim ini mengingat gelar Liga Inggris sulit diraih karena masih tertinggal jauh dari Manchester City. Oleh karena itu pelatih asal Portugal itu harus menurunkan pemain terbaiknya saat menghadapi Huddersfield Town pada pertandingan putaran kelima, di John Smith ’s Stadium, Minggu (18 / 2 / 2018) dini hari WIB. Hasilnya MU menang 2 - 0 dan bakal lolos ke perempat final. Dan Romelu Lukaku yang jadi pahlawa Setan Merah dengan dua golnya masing-masing menit ketiga dan menit ke - 55. Dan MU akan menghadapi tim yang relatif mudah di perempat final yaitu Brighton. Sedangkan Chelsea harus bertemu dengan Leicester City. Tentu laga sulit bagi kedua tim penghuni Liga Inggris itu. Mourinho memang tidak salah menurunkan skuad terbaiknya. Buktinya upaya tersebut membuahkan hasil saat pertandingan baru berjalan tiga menit Man United sudah unggul duluan. Menerima umpan Juan Mata, Romelu Lukaku melepaskan tendangan kaki kanan untuk mengubah kedudukan menjadi 1 - 0. MU terus mencoba mencetak gol tambahan namun selalu gagal sehingga babak pertama berakhir dengan kedudukan 1 - 0. Pada babak kedua, tim tuan rumah mencoba membalas. Pada menit ke - 47, Philip Billing mendapatkan kesempatan, namun bola tendangannya masih dapat diantisipasi kiper Manchester United, Sergio Romero Justru menit ke - 55, Manchester United menambah keunggulan menjadi 2 - 0. Lukaku kembali mencatatkan nama di papan skor setelah menerima umpan Alexis Sanchez melalui skema serangan balik. Tertinggal dua gol, tim tuan rumah mencoba membalas. Pada menit-menit akhir, Huddersfield terus mengurung pertahanan Manchester United. Namun, beberapa peluang yang mereka peroleh gagal dikonversi menjadi gol. Skor 2 - 0 untuk Manchester United pun bertahan hingga pertandingan usai. (b)']</t>
         </is>
       </c>
     </row>
@@ -520,21 +520,21 @@
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>2284</v>
+        <v>2124</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>1_jakarta_kpk_jalan_indonesia</t>
+          <t>1_jakarta_kpk_ketua_tersangka</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>['jakarta', 'kpk', 'jalan', 'indonesia', 'polisi', 'ketua', 'tersangka', 'dki', 'orang', 'partai']</t>
+          <t>['jakarta', 'kpk', 'ketua', 'tersangka', 'indonesia', 'jalan', 'partai', 'polisi', 'orang', 'pelaku']</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>['Rimanews - Polisi dan TNI akan menjaga ketat kotak suara mulai dari tingkat TPS hingga rapat pleno rekapitulasi hasil perhitungan suara digelar di KPU DKI Jakarta. " Pokoknya melekat terus sampai nanti ke KPU provinsi, kemudian nanti penghitungan pun kita jaga dan dikawal semua, " kata Kepala Bidang Humas Polda Metro Jaya Komisaris Besar Polisi Argo Yuwono di Jakarta, hari ini. Argo mengatakan, saat ini, aparat mengawal kotak suara bersama Petugas Pemilihan Kecamatan (PPK), kemudian akan dibawa ke KPU kota hingga KPU provinsi. Argo mengapresiasi masyarakat Jakarta yang ikut menjaga situasi dan kondisi di ibu kota tetap aman selama Pilkada DKI Jakarta putaran kedua 2017. Argo menyebutkan terjadi beberapa insiden kecil saat pencoblosan pada sejumlah wilayah, namun dapat diselesaikan termasuk sekelompok massa yang mendekati TPS telah dipulangkan ke daerahnya. DKI Jakarta menggelar Pilkada putaran kedua yang diikuti pasangan calon Basuki Tjahaja Purnama alias Ahok - Djarot Saiful Hidayat dan Anies Baswedan - Sandiaga Uno, kemarin. Berdasarkan hitung cepat sejumlah lembaga survei Anies - Sandi menang dengan perolehan suara 58 persen sementara Ahok - Djarot hanya meraih 42 persen.', 'Jakarta (ANTARA News) - Ketua Komisi Pemberantasan Korupsi (KPK) menyatakan tidak menargetkan waktu terkait pelimpahan berkas perkara tersangka kasus korupsi KTP - elektronik (KTP - e) Setya Novanto ke tahap penuntutan. " Kami tidak menargetkan tetapi yang pasti saat berkasnya sudah siap, ya akan dilimpahkan, " kata Kabag Pemberitaan dan Publikasi KPK Priharsa Nugraha di gedung KPK, Jakarta, Selasa. Ia pun menegaskan bahwa sampai saat ini lembaganya belum melimpahkan berkas perkara Novanto ke tahap penuntutan. " Hingga kini belum dilakukan pelimpahan ke pengadilan, " kata Priharsa. Sebelumnya sempat beredar informasi yang menyebutkan bahwa berkas perkara Novanto sudah dilimpahkan ke pengadilan. " Yang perlu dipahami adalah proses di KPK karena penyidik dan Jaksa Penuntut Umum berada dalam satu atap telah terjadi koordinasi sebelumnya, artinya saat penyidikan itu dimulai juga telah ada P16 yang menunjuk tim Jaksa Peneliti yang akan mendampingi proses penyidikan, " tuturnya. Sebelumnya, Wakil Ketua KPK Basaria Panjaitan menyatakan bahwa berkas perkara Novanto sudah selesai. Namun, KPK masih menunggu beberapa saksi dan ahli meringankan Novanto yang belum diperiksa sehingga berkas perkara belum dilimpahkan ke penuntut umum. " Berkas penyidikan sudah selesai, karena itu hak dia untuk minta saksi-saksi meringankan, untuk itu kami harus melakukan pemeriksaan, " kata Basaria di gedung KPK, Jakarta, Rabu (29 / 11). Setya Novanto ditetapkan kembali menjadi tersangka kasus korupsi KTP - e pada Jumat (10 / 11). Setya Novanto selaku anggota DPR RI periode 2009 - 2014 bersama-sama dengan Anang Sugiana Sudihardjono, Andi Agustinus alias Andi Narogong, Irman selaku Direktur Jenderal Kependudukan dan Pencatatan Sipil Kemendagri dan Sugiharto selaku Pejabat Pembuat Komitment (PPK) Dirjen Dukcapil Kemendagri dan kawan-kawan diduga dengan tujuan menguntungkan diri sendiri atau orang lain atau suatu koporasi, menyalahgunakan kewenangan kesempatan atau sarana yang ada padanya karena jabatan atau kedudukan sehingga diduga mengakibatkan kerugian keuangan negara atas perekonomian negara sekurangnya Rp 2,3 triliun dari nilai paket pengadaan sekitar Rp 5,9 triliun dalam pengadaan paket penerapan KTP - E 2011 - 2012 Kemendagri. Setya Novanto disangkakan pasal 2 ayat 1 subsider pasal 3 UU No 31 tahun 1999 tentang Pemberantasan Tindak Pidana Korupsi sebagaimana telah diubah dengan UU No 20 tahun 2001 tentang perubahan atas UU No 31 tahun 1999 tentang Pemberantasan Tindak Pidana Korupsi jo pasal 55 ayat 1 ke - 1 KUHP. Saat ini, Novanto juga telah mengajukan permohonan praperadilan di Pengadilan Negeri Jakarta Selatan. Sidang perdana akan digelar pada Kamis (7 / 12) setelah sebelumnya sempat ditunda selama satu pekan.', 'Jakarta, CNN Indonesia - - Komisi Pemberantasan Korupsi (KPK) resmi menetapkan Ketua DPR Setya Novanto sebagai tersangka kasus korupsi pengadaan proyek e - KTP. Penetapan status tersangka yang kedua kalinya ini disampaikan Wakil Ketua KPK Saut Situmorang. " KPK menerbitkan surat perintah penyidikan pada 31 Oktober 2017 atas nama tersangka SN (Setya Novanto), Ketua DPR RI, " kata \xa0 Saut \xa0 di Gedung KPK, Jakarta, Jumat (10 / 11). Sebelumnnya, surat pemberitahuan dimulainya penyidikan (SPDP) beredar di kalangan wartawan. SPDP \xa0 itu \xa0 diantarkan ke rumah tersangka \xa0 pada 3 November 2017. Namun saat itu KPK belum memberikan keterangan resmi terkait penetapan Novanto sebagai tersangka. Surat itu ditandatangani oleh Direktur Penyidikan KPK, Aris Budiman. Di dalamnya menyebutkan, penyidikan kasus dugaan korupsi e - KTP dengan tersangka Novanto sudah dimulai sejak 31 Oktober 2017. Novanto diduga melakukan korupsi bersama Anang Sugiana Sudiharjo, Andi Agustinus, Andi Narogong, Irman, dan Sugiharto. Novanto dijerat dengan Pasal 2 ayat 1 subsider Pasal 3 Undang-Undang Nomor 31 tahun 1999 sebagaimana diubah dengan Undang-Undang Nomor 20 tahun 2001 tentang Pemberantasan Korupsi (UU Tipikor) juncto Pasal 55 ayat 1 ke - 1 KUHP. Ini kali kedua KPK menetapkan Novanto sebagai tersangka kasus dugaan korupsi e - KTP. Sebelumnya, pada 17 Juli 2017, KPK menetapkan Novanto sebagai tersangka dalam kasus yang sama. Setelah penetapan itu, Novanto selalu mangkir dari panggilan KPK dengan alasan sakit. Dia sempat dirawat di RS Siloam Semanggi, sebelum akhirnya dipindahkan ke RS Premier Jatinegara. Novanto pun mengajukan praperadilan ke Pengadilan Negeri Jakarta Selatan. Majelis Hakim Tunggal, Cepi Iskandar dalam amar putusannya menyatakan \xa0 penetapan tersangka Novanto oleh KPK tidak sah. Dia pun bebas dari jerat hukum. (pmg / sur)']</t>
+          <t>['Jakarta, CNN Indonesia - - Komisi Pemberantasan Korupsi (KPK) resmi menetapkan Ketua DPR Setya Novanto sebagai tersangka kasus korupsi pengadaan proyek e - KTP. Penetapan status tersangka yang kedua kalinya ini disampaikan Wakil Ketua KPK Saut Situmorang. " KPK menerbitkan surat perintah penyidikan pada 31 Oktober 2017 atas nama tersangka SN (Setya Novanto), Ketua DPR RI, " kata \xa0 Saut \xa0 di Gedung KPK, Jakarta, Jumat (10 / 11). Sebelumnnya, surat pemberitahuan dimulainya penyidikan (SPDP) beredar di kalangan wartawan. SPDP \xa0 itu \xa0 diantarkan ke rumah tersangka \xa0 pada 3 November 2017. Namun saat itu KPK belum memberikan keterangan resmi terkait penetapan Novanto sebagai tersangka. Surat itu ditandatangani oleh Direktur Penyidikan KPK, Aris Budiman. Di dalamnya menyebutkan, penyidikan kasus dugaan korupsi e - KTP dengan tersangka Novanto sudah dimulai sejak 31 Oktober 2017. Novanto diduga melakukan korupsi bersama Anang Sugiana Sudiharjo, Andi Agustinus, Andi Narogong, Irman, dan Sugiharto. Novanto dijerat dengan Pasal 2 ayat 1 subsider Pasal 3 Undang-Undang Nomor 31 tahun 1999 sebagaimana diubah dengan Undang-Undang Nomor 20 tahun 2001 tentang Pemberantasan Korupsi (UU Tipikor) juncto Pasal 55 ayat 1 ke - 1 KUHP. Ini kali kedua KPK menetapkan Novanto sebagai tersangka kasus dugaan korupsi e - KTP. Sebelumnya, pada 17 Juli 2017, KPK menetapkan Novanto sebagai tersangka dalam kasus yang sama. Setelah penetapan itu, Novanto selalu mangkir dari panggilan KPK dengan alasan sakit. Dia sempat dirawat di RS Siloam Semanggi, sebelum akhirnya dipindahkan ke RS Premier Jatinegara. Novanto pun mengajukan praperadilan ke Pengadilan Negeri Jakarta Selatan. Majelis Hakim Tunggal, Cepi Iskandar dalam amar putusannya menyatakan \xa0 penetapan tersangka Novanto oleh KPK tidak sah. Dia pun bebas dari jerat hukum. (pmg / sur)', 'Jakarta, CNN Indonesia - - Komisi Pemberantasan Korupsi (KPK) meminta Ketua DPR Setya Novanto memenuhi panggilan penyidik untuk diperiksa selaku tersangka korupsi proyek pengadaan e - KTP. KPK akan memanggil Setnov, Rabu (15 / 11) dan surat panggilan untuk Ketua Umum Partai Golkar itu sudah dikirimkan pekan lalu. " Saya kira ini seharusnya menjadi bentuk kepatuhan kita terhadap hukum. Kalau kemudian dipanggil oleh penegak hukum sebaiknya datang, " kata Juru Bicara KPK Febri Diansyah di Gedung KPK, Jakarta, Selasa (14 / 11). Febri menyebut, pemeriksaan ini seharusnya dijadikan Setnov sebagai ruang klarifikasi dalam kasus korupsi yang ditaksir merugikan negara hingga Rp 2,3 triliun. Terlebih, kata Febri, fakta-fakta baru sudah muncul di persidangan Andi Agustinus alias Andi Narogong yang semakin menguatkan konstruksi hukum kasus e - KTP. " Sebenarnya ini harus dilihat juga sebagai kesempatan atau ruang untuk memberikan klarifikasi lebih lanjut, " ujar Febri. Menurut Febri, alasan ketidakhadiran Setnov saat dipanggil sebagai saksi dengan menyebut KPK perlu mengantongi izin Presiden Joko Widodo dan memiliki hak imunitas, tak beralasan berdasarkan hukum. " Kita baca secara lebih lengkap UU MD3 tersebut, ada penegasan pengecualian izin tertulis presiden itu jika disangkakan melanggar tindak pidana khusus. Artinya, klausul itu tidak bisa digunakan lagi, " tuturnya. Febri belum mau berandai-andai apakah penyidik KPK akan langsung menahan mantan Ketua Fraksi Golkar itu jika besok memenuhi panggilan selaku tersangka. KPK, lanjutnya juga belum berencana menjemput paksa Setnov. " Kita belum bicara tentang penahanan juga. Karena agendanya pemanggilan dan pemeriksaan sebagai tersangka, " kata dia (wis / djm)', 'JAKARTA (Pos Kota) – Penyidik Direktorat Lalu Lintas (Ditlantas) Polda Metro Jaya melakukan pemeriksaan terhadap Ketua DPR RI, Setya Novanto, terkait insiden kecelakaan tunggal yang dialami di Jalan Permata Berlian, Permata Hijau, Kebayoran Lama, Jakarta Selatan, Kamis malam pekan lalu. Ketua Umum Partai Golkar ini diperiksa sebagai saksi untuk tersangka Hilman Mattauch. “ Iya sebagai saksi korban atas kejadian pada hari Kamis tanggal 16 November pukul 18.30, dengan tersangka inisial HM (Hilman Mattauch), ” kata Dirlantas Polda Metro Jaya, Kombes Pol Halim Pagarra, di Gedung KPK Merah Putih, Jalan Kuningan Persada, Setiabudi, Jakarta Selatan, Kamis (23 / 11 / 2017). Menurutnya, ada beberapa pertanyaan yang akan penyidik Ditlantas Polda Metro Jaya konfirmasi kepada Novanto. Salah satunya soal kronologis sebelum mobil yang dia tumpangi menabrak tiang listrik. “ Sebenernya ada pertanyaan wajib bagaimana dia apakah dalam keadaan sehat, siap diperiksa, didampingi oleh pengacara dan juga apa yang diketahui beliau yang dia lihat itu yang akan kita tanyakan, ” ujarnya. Halim menambahkan, pihaknya pun telah memperoleh izin dari KPK untuk memeriksa Novanto di Gedung KPK. Selain berstatus tersangka kasus korupsi KTP elektronik, Novanto pun telah menjadi tahanan KPK. “ Sehat jadi kita kirim surat ke Ketua KPK untuk memeriksa korban ini. (Korban) siap hari ini, ” imbuhnya. Sebagaimana diketahui, Novanto kembali ditetapkan tersangka dalam kasus korupsi e - KTP pada 10 November 2017. Dia diduga menyalahgunakan kewenangannya sehingga negara disinyalir dirugikan hingga Rp 2,3 triliun. Ini merupakan kali kedua Novanto ditetapkan sebagai tersangka oleh KPK. Ia sebelumnya menjadi tersangka dalam kasus korupsi e - KTP. Namun, status tersangkanya gugur karena menang praperadilan melawan KPK. Usai ditetapkan kembali sebagai tersangka, Novanto sempat menghilang. Beberapa hari kemudian, ia mengalami kecelakaan. Mobil yang ditumpanginya menabrak tiang listrik di kawasan Permata Hijau, Jakarta Selatan. Akibatnya, Ketua Umum Partai Golkar nonaktif itu dilarikan ke Rumah Sakit Medika Permata Hijau dan dipindahkan ke RSCM. KPK kemudian bergerak cepat dan menahan Novanto. Kini dia berada dalam Rutan KPK. Meski telah mengenakan rompi oranye, Novanto tak tinggal diam. Melalui kuasa hukumnya, dia berencana mengajukan kembali praperadilan. Rencananya, praperadilan Novanto yang kedua digelar pada 30 November di Pengadilan Negeri Jakarta Selatan. Selain praperadilan, pria yang akrab disapa Setnov itu juga meminta perlindungan kepada Presiden Joko Widodo dan Komisi III DPR. (julian / yp)']</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>1281</v>
+        <v>1268</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -555,12 +555,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>['film', 'lagu', 'album', 'konser', 'indonesia', 'jakarta', 'anak', 'orang', 'musik', 'sang']</t>
+          <t>['film', 'lagu', 'album', 'konser', 'indonesia', 'jakarta', 'orang', 'anak', 'musik', 'sang']</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>['Jakarta, CNN Indonesia - - Edwin, sutradara asal Indonesia baru saja memenangkan Busan Award di Asian Project Market (APM), yang berlangsung 9 - 11 Oktober 2016 di Busan, Korea Selatan. Kali ini, sutradara yang pernah membuat film Babi Buta yang Ingin Terbang (2008) itu membawa proyek film Seperti Dendam, Rindu Harus Dibayar Tuntas, yang diadaptasi dari novel ketiga Eka Kurniawan. Dalam penulisan skenarionya, Edwin berkolaborasi dengan Eka. " Buku Eka Kurniawan ini sangat visual. Bahkan beberapa bagian cerita didalamnya, terasa ada baunya, " ujar Edwin beralasan, seperti pernyataan yang dikirimkannya, pada Kamis (13 / 10). Lebih jauh, ia mengatakan bahwa novel Eka juga sangat kental dengan pengetahuan, dan segenap misteri yang mempengaruhi pembentukan kebudayaan modern masyarakat. " Seperti jutaan anak laki-laki di Jawa yang \xa0  tumbuh di era tahun 1980an, saya sangat mengenali Ajo Kawir dan dunianya. Dunia di mana dangdut pantura mengiringi rasa rindu para supir truk yang bergelut sehari-hari dengan machismo atau maskulinitas, dan adrenalin ”, kata sutradara kelahiran Surabaya itu. Film berkualitas Palari Films membawa Seperti Dendam, Rindu Harus Dibayar Tuntas (judul internasional: Vengeance Is Mine, All Others Pay Cash) ke Asian Project Market yang selama 19 tahun telah konsisten menyeleksi dan mempertemukan proyek film berkualitas kepada pendana, investor film, dan pembeli film dari berbagai negara. Tahun 2016 ini, APM memilih 27 proyek film dari 16 negara. Proses seleksi yang ketat menjamin kualitas artistik dan keragaman tema film - film yang dijajakan di APM. Film - film blockbuster seperti Snowpiercer karya Bong Joon - ho, maupun film - film unik seperti Stray Dogs karya Tsai Ming Liang bisa terwujud karena film - film tersebut bertemu dengan pasarnya yang tepat. Snowpiercer berjaya di Hollywood, Stray Dogs memenangkan Grand Jury Prize di Venice Film Festival. Film Seperti Dendam, Rindu Harus Dibayar Tuntas adalah proyek kolaborasi pertama Edwin dan Eka Kurniawan. Film terakhir Edwin, Postcards From The Zoo, adalah film Indonesia pertama yang terseleksi dan dinominasikan sebagai film panjang terbaik oleh Berlin International Film Festival (Berlinale 2012). Sementara Eka Kurniawan baru saja memenangkan OppenheimerFunds Emerging Voices 2016 Fiction Award untuk novelnya, Manusia Harimau (Man Tiger). Eka juga pernah dinominasikan untuk Man Booker Prize International dengan novel yang sama. Sebelumnya, dia juga telah memenangkan World Reader ’s Award 2016 untuk novel pertamanya Cantik itu Luka (Beauty is A Wound). Seperti Dendam, Rindu Harus Dibayar Tuntas, adalah novel ketiga dan selain difilmkan, novel ini rencananya akan diterbitkan di Amerika Serikat, pertengahan tahun 2017. Muhammad Zaidy, salah satu produser dari Palari Films, melihat potensi luar biasa dari buku ketiga Eka Kurniawan ini sebagai materi yang kuat untuk diolah menjadi film. “ Namun seperti kita ketahui, mengadaptasi sebuah novel ke film, bukan pekerjaan yang mudah. Perlu visi yang sejalan antara sang penulis novel, dan pembuat filmnya. Kami baru bisa yakin dengan proyek adaptasi film ini setelah mempertemukan Eka Kurniawan dengan Edwin, " ujarnya. Zaidy menambahkan, visi Edwin terhadap film, dan pemahamannya terhadap novel Eka, membuat ia bersemangat dan percaya bahwa proyek film ini harus dikerjakan. " Kita akan membuat film yang menghibur, indah dan unik baik secara kemasan maupun isi cerita, ” tutur pria kelahiran Makassar, yang baru-baru ini juga terlibat memproduksi film Athirah, dan AADC?2. Dengan film ini Palari Films berharap mampu membuka minat berbagai macam kalangan terhadap film Indonesia, memperluas pasar film Indonesia baik di dalam negeri maupun di luar negeri. Meiske Taurisia, juga produser dari proyek film ini menambahkan, “ Pasar Film Indonesia perlu terus digali. Kami para produser film Indonesia terus mengolah kreatifitas untuk menyuguhkan berbagai pilihan tontonan film Indonesia kepada masyarakat . " Ia menambahkan, semakin banyak pilihan bentuk dan cerita pada film Indonesia, maka semakin banyak peluang untuk memperkaya penonton dan pasar film Indonesia. Meiske pernah menangani film Postcards From The Zoo \xa0 yang disutradarai Edwin, hingga kemudian dibeli hak edarnya oleh distributor film internasional dari Perancis, Inggris, Jerman, Korea Selatan, dan Taiwan. (rah)', 'Jakarta, CNN Indonesia - - Setelah sukses menjadi penyanyi dan pencipta lagu, Ed Sheeran belum juga puas berkarya. Ia bakal mencoba peruntungan di dunia layar lebar. Sheeran berencana membuat sebuah film lengkap dengan soundtrack yang berasal dari lagu-lagu miliknya. Melansir NME, Ed Sheeran sudah membicarakan proyek film itu dengan para pembuat film. " Saya sedang melakukan pembicaraan dengan salah satu pembuat film yang sangat saya kagumi dan kami akan membuatnya pelan tapi pasti, " kata Sheeran kepada The Sun. Penyanyi yang baru saja merilis album ÷ [Devide] itu menjelaskan, film itu akan dibuat dengan bujet rendah, independen dan berkarakter Inggris. Bukan hanya merencanakan film dan lagu - lagunya, Sheeran juga mengaku ingin bermain di film yang ia buat sendiri itu. " Saya sangat ingin membuat sebuah film, saya membuat soundtrack -nya dan bermain di film itu. Itu adalah rencana saya selanjutnya, " kata pelantun lagu Shape of You itu. Soal film, Sheeran menjadikan Notting Hill (1999) dan Once (2007) sebagai acuan sekaligus inspirasinya. Notting Hill merupakan film komedi romantis Inggris yang dibintangi Julia Roberts dan Hugh Grant. Sementara Once adalah film drama musikal romantis dari Irlandia. " Saya melihat film Notting Hill dan saya pikir itu merupakan patokan yang tepat, atau Once. Jika menggabungkan Notting Hill dengan Once, saya akan bilang ini akan menjadi awal yang baik, " tuturnya. Penyanyi Thinking Out Loud itu juga akan mengisi film dengan lagu pengiring yang berasal dari tembang yang dimilikinya. Kendati demikian, Sheeran tak akan membuat lagu-lagu itu sebagai album khusus. " Saya tidak berpikir akan menjadikan album untuk soundtrack itu, tapi saya pasti akan meletakkan lagu-lagu saya di situ, tapi tidak akan menjadi album, " ujar Sheeran yang selama ini menggunakan lambang matematika untuk setiap judul albumnya. Sheeran memang belakangan aktif kembali, setelah setahun belakangan tak banyak muncul ke hadapan publik. Sekali muncul, ia seakan tak kehabisan rencana. Beberapa waktu lalu sahabat Taylor Swift itu mengungkapkan tengah membuat boyband yang dijuluki\' Superpop’. " Saya akan membentuk tiga sampai empat laki-laki dalam boyband, lalu membawa mereka ikut dalam tur bersama saya, " ujarnya. (rsa / rsa)', 'Film\' Susah Sinyal\' karya sutradara Ernest Prakasa telah dirilis sejak 21 Desember 2017. Hanya dalam waktu 9 hari saja, film yang bergenre drama komedi tersebut telah berhasil meraih satu juta penonton, lebih tepatnya 1.042.309 penonton. Informasi tersebut diketahui melalui keterangan tertulis yang diterima oleh kumparan (kumparan.com) pada Sabtu (30 / 12). Ini merupakan sebuah pencapaian yang menggembirakan bagi Ernest dan sang istri, Meira Anastasia, yang juga terlibat dalam penulisan naskah film ini. Pasangan yang menikah pada tahun 2007 ini mengaku sangat bahagia, karena kerja keras mereka akhirnya mendapatkan sambutan yang luar biasa dari para penikmat film Indonesia. Sebelumnya, jaringan bioskop terbesar di Indonesia, yakni XXI, juga memberikan pengumuman menggembirakan ini melalui media sosial Twitter milik mereka. " Selamat kepada @ernestprakasa dan @Starvisionplus atas raihan 1 juta penonton #SusahSinyalMovie yang sedang tayang di bioskop, " tulis akun @cinemaxxi. Ernest pun mengutarakan rasa bahagianya tersebut lewat sebuah postingan di Instagram di akun @ernestprakasa. " Gw seneng karena @susahsinyalmovie tembus 1 juta penonton, tapi lebih seneng lagi karena ini menandakan bahwa perfilman Indonesia 2017 berhasil mengulang prestasi gemilang tahun lalu, yakni 10 film teratas dengan penonton lebih dari 1 juta. Terimakasih sudah percaya sama film Indonesia walau harga tiketnya sama kayak film Hollywood. Tanpa dukungan kamu, kami nggak akan punya ruang untuk bertumbuh. Bangga film Indonesia! #SusahSinyalMovie, " tulisnya dalam kolom keterangan. Jumlah penonton film\' Susah Sinyal\' ini berada di bawah jumlah penonton film\' Ayat - ayat Cinta 2\', yang berhasil menyedot 1.581.567 penonton, ke bioskop dalam 8 hari penayangannya. Meskipun berbeda genre, namun kedua film ini dirilis di hari yang bersamaan. \' Susah Sinyal\' merupakan film ketiga yang diciptakan oleh pria berusia 35 tahun tersebut. Sebelumnya, ia telah merilis film yang berjudul\' Ngenest\' di tahun 2015 dan\' Cek Toko Sebelah\' di tahun 2016. Kedua film tersebut juga dirilis setiap bulan Desember dan sama-sama mendapatkan beberapa penghargaan. Bagi Ernest, fenomena ini adalah bukti bahwa drama komedi adalah genre film yang tidak bergantung pada musim, dan film komedi yang dibuat dengan baik, pasti akan selalu mendapat apresiasi dari masyarakat. Hingga saat ini, promosi film\' Susah Sinyal\' masih akan terus diusahakan oleh Ernest dan segenap timnya. Roadshow yang telah dilakukan ke berbagai kota di Indonesia, seperti Jakarta, Bandung, Cikarang, Karawang, Bekasi, Palembang, dan Medan pun mendapatkan sambutan hangat dari penonton lokal. Film\' Susah Sinyal\' menceritakan tentang sosok Ellen (Adinia Wirasti), seorang pengacara sukses sekaligus orang tua tunggal. Ia memiliki seorang putri, bernama Kiara (Aurora Ribero), berusia 17 tahun yang memiliki watak pemberontak. Hubungan keduanya tak akur karena Ellen tak pernah punya waktu untuk Kiara. Keributan antara ibu dan anak ini akhirnya membuat ibunda Ellen, Agatha (Niniek L Karim), terkena serangan jantung, dan membuat mereka berdua terpukul. Peristiwa itu kemudian membawa Ellen dan Kiara ke sebuah perjalanan ke Sumba, Nusa Tenggara Timur, untuk memperbaiki hubungan mereka.']</t>
+          <t>['Jakarta, CNN Indonesia - - Film horor Indonesia saat ini tampak mengalami perubahan. Tak ada lagi wanita seksi yang sempat menjadi bahan utama film horor seperti beberapa tahun lalu. Justru, film horor lawas mulai bangkit kembali dengan kualitas yang boleh diadu. Bukan tanpa alasan para produser film mulai mengangkat kembali film horor dari berdekade - dekade silam dengan teknologi perfilman terbaru. Sunil Samtani, produser Rapi Films, saat berbincang dengan CNNIndonesia.com beberapa waktu lalu menyebut beberapa alasan ia kembali mengangkat film horor lawas. Di antaranya, konsep yang kuat dan tren sineas yang mulai peduli akan kualitas. " Ada beberapa proyek [film lawas] yang kalau di - remake pasti bagus. Misalnya Jelangkung (2001), karena itu kuat sekali. Namun juga tidak semua film bisa di - remake karena seberapa kuat konsepnya? " kata Sunil. Rapi Films tergolong rumah produksi yang telah menghasilkan banyak film horor di masa lalu, sebut saja film Sundel Bolong (1981) yang ikonis dengan Suzzanna memesan 200 tusuk sate, dan Pengabdi Setan (1980) yang kini digarap lagi oleh Joko Anwar. Di era modern, Sunil sempat bereksperimen dengan sejumlah film horor untuk menyesuaikan tren zaman, seperti Kereta Hantu Manggarai (2008), Rumah Hantu Ampera (2009), hingga Kuntilanak Kesurupan (2011). Namun, dari sekian banyak koleksi film horor yang telah dibuat perusahaan yang didirikan oleh sang ayah, Gope T Samtani itu, Sunil mengakui bahwa film lawas memiliki sejumlah keunggulan meski film horor era modern pun banyak juga yang berkualitas baik. " Kalau dilihat, film lawas itu lebih menakutkan, lebih terasa akrab, CGI pun belum ada sehingga yang mereka buat itu lebih nyata, " kata Sunil. " Saat ini CGI banyak sekali . " " Namun film saat ini seperti The Conjuring, CGI yang digunakan banyak namun tetap laris. Berarti menurut saya, tergantung konsep cerita dan pendekatan ke penonton. Kalau bagus, ya jalan saja, " lanjutnya. Kekuatan konsep pula yang disebut Sunil jadi alasan mengangkat kembali Pengabdi Setan dan mempercayakan kepada Joko Anwar untuk mengangkat kembali teror arwah seorang ibu kepada keluarganya itu. Pengabdi Setan, diklaim Sunil, sempat mendapatkan banyak apresiasi dari berbagai pihak dan disebut sebagai film horor terseram di Indonesia. Meski berdalih akan kekuatan konsep, menurut pengamat film Adrian Pasaribu, dibuat atau diangkatnya kembali film horor lawas di era modern adalah karena faktor ekonomi. " Kenapa film horor lawas mulai dibuat remake atau diangkat kembali? Mungkin jawabannya lebih simpel: ekonomi, " kata Adrian saat berkorespondensi dengan CNNIndonesia.com, dalam kesempatan terpisah. " Dalam remake film horor lawas, ada satu faktor lagi yang mungkin bisa menguntungkan si pembuat: basis penonton, " kata Adrian. Menurut Adrian, film berseri baik dalam bentuk remake, reboot, sekuel, maupun prekuel, akan bergantung pada basis penonton yang terbentuk dari film aslinya. Pembuatan seri lain yang masih berhubungan dengan film asli setidaknya sudah punya penonton, yakni penggemar seri terdahulunya. Jumlah penonton bisa bertambah jika sutradara mampu menggaet\' pasar\' baru. Di sisi lain, Adrian meyakini film horor tergolong genre gambar bergerak yang tidak terlalu membutuhkan biaya besar seperti drama atau genre lainnya. Asumsi ini terlihat dari biaya produksi film horor Hollywood, seperti The Conjuring dari Warner Bros. pada 2013. Film garapan James Wan itu dibuat dengan bujet US$20 juta namun mendapat penghasilan hingga US$318 juta atau untung lebih dari 15 kali lipat. Hal ini berbeda dengan karya Warner Bros. lainnya di tahun yang sama, Man of Steel. Film ini membutuhkan bujet US$225 juta namun hanya mendapatkan penghasilan sebesar US$668 juta atau dua kali lipat dari biaya produksi. " Kasarnya, sudah ada perkiraan jaminan penonton, " kata Adrian. " Nah, coba perhitungkan dua unsur itu: biaya produksi murah plus jaminan penonton. Klop sudah . " Namun dua hal itu ternyata belum cukup memenangi hati para produser untuk membuat film horor di era modern. Sunil mengakui, masuknya genre horor Hollywood seperti The Conjuring yang memiliki konsep kuat adalah tantangan bagi sineas di Indonesia. " Karena setiap tahun penonton dapat film Hollywood macam The Conjuring, Insidious yang smart horror secara kualitas, lama-lama penonton akan membandingkannya dengan produksi Indonesia, " kata Sunil.', 'Jakarta, CNN Indonesia - - Setelah sukses menjadi penyanyi dan pencipta lagu, Ed Sheeran belum juga puas berkarya. Ia bakal mencoba peruntungan di dunia layar lebar. Sheeran berencana membuat sebuah film lengkap dengan soundtrack yang berasal dari lagu-lagu miliknya. Melansir NME, Ed Sheeran sudah membicarakan proyek film itu dengan para pembuat film. " Saya sedang melakukan pembicaraan dengan salah satu pembuat film yang sangat saya kagumi dan kami akan membuatnya pelan tapi pasti, " kata Sheeran kepada The Sun. Penyanyi yang baru saja merilis album ÷ [Devide] itu menjelaskan, film itu akan dibuat dengan bujet rendah, independen dan berkarakter Inggris. Bukan hanya merencanakan film dan lagu - lagunya, Sheeran juga mengaku ingin bermain di film yang ia buat sendiri itu. " Saya sangat ingin membuat sebuah film, saya membuat soundtrack -nya dan bermain di film itu. Itu adalah rencana saya selanjutnya, " kata pelantun lagu Shape of You itu. Soal film, Sheeran menjadikan Notting Hill (1999) dan Once (2007) sebagai acuan sekaligus inspirasinya. Notting Hill merupakan film komedi romantis Inggris yang dibintangi Julia Roberts dan Hugh Grant. Sementara Once adalah film drama musikal romantis dari Irlandia. " Saya melihat film Notting Hill dan saya pikir itu merupakan patokan yang tepat, atau Once. Jika menggabungkan Notting Hill dengan Once, saya akan bilang ini akan menjadi awal yang baik, " tuturnya. Penyanyi Thinking Out Loud itu juga akan mengisi film dengan lagu pengiring yang berasal dari tembang yang dimilikinya. Kendati demikian, Sheeran tak akan membuat lagu-lagu itu sebagai album khusus. " Saya tidak berpikir akan menjadikan album untuk soundtrack itu, tapi saya pasti akan meletakkan lagu-lagu saya di situ, tapi tidak akan menjadi album, " ujar Sheeran yang selama ini menggunakan lambang matematika untuk setiap judul albumnya. Sheeran memang belakangan aktif kembali, setelah setahun belakangan tak banyak muncul ke hadapan publik. Sekali muncul, ia seakan tak kehabisan rencana. Beberapa waktu lalu sahabat Taylor Swift itu mengungkapkan tengah membuat boyband yang dijuluki\' Superpop’. " Saya akan membentuk tiga sampai empat laki-laki dalam boyband, lalu membawa mereka ikut dalam tur bersama saya, " ujarnya. (rsa / rsa)', 'Jakarta, CNN Indonesia - - Film laga bertema sejarah Korea, The Battleship Island berhasil menarik 5 juta penonton, meski tersandung beberapa kontroversi di Negeri Ginseng. Di balik sejumlah kontroversi yang menyelimutinya, The Battleship Island malah berhasil menjadi film tercepat di Korea yang meraih lima juta penonton tahun ini. Film itu berhasil mengalahkan Spider - Man: Homecoming dengan tiga hari lebih cepat mendapatkan lima juta penonton di Negeri Ginseng. Distributor film The Battleship Island, CJ Entertainment mengunggah foto ucapan terima kasih kepada para penonton di akun resmi Instagram mereka. Dalam foto itu, tampak lima bintang utama, yakni Song Joong Ki, So Ji Sub, Hwang Jung Min, Lee Jung Hyun, dan Kim Su An memegang tulisan besar bertuliskan lima juta penonton. Diberitakan Digital Times via Naver, CJ Entertainment mengungkapkan, film garapan Ryu Seung Wan itu tersebut mencetak rekor baru dengan penonton yang mencapai 970 ribu pada malam pertama (26 / 7) penayangannya. Di hari ke - dua, jumlah penonton The Battleship Island mencapai satu juta dan terus bertambah menjadi empat juta penonton setelah lima hari dirilis dan meraup sekitar Rp 372 miliar dari penjualan tiket. Padahal, film itu dibuat dengan modal 23 miliar won atau sekitar Rp 273 miliar. Di hari ke - enam, film dengan bujet termahal di Korea Selatan itu mencatatkan rekor lima juta penonton. Selain itu, film ini juga memecahkan rekor sutradara Ryu Seung Wan yang sebelumnya juga memperoleh lima juta penonton, yakni Veteran dan Assassination. Sementara itu, aktor kondang So Ji Sub pernah menyatakan dia berharap film ini ditonton lebih dari 10 juta orang. “ Saya berharap dapat lebih dari 10 juta orang. Ini harus memecahkan angka tersebut agar film sejenis ini dapat tetap dibuat di masa depan. Saya juga berharap mereka yang sudah bekerja keras dalam film ini dapat diapresiasi, ” ujarnya. Selain jumlah penonton yang tinggi, film ini juga diwarnai kontroversi. Pasalnya, Hashima, pulau yang dijadikan sejarah pembuatan film ini masuk dalam situs bersejarah UNESCO tanpa adanya data sejarah yang lengkap. Orang Korea pun banyak menyebut film ini tak sesuai dengan fakta sejarah. Menurut mereka, The Battleship Island malah menonjolkan permasalahan antarorang Korea sendiri yang saling berkhianat satu dengan lainnya. Selain itu, film ini juga membahas lebih banyak soal orang Korea yang pro - Jepang pada masa itu. Dalam film berlatar Perang Dunia II itu, Song Joong Ki berperan sebagai Park Moo Young, anggota pergerakan kemerdekaan Korea ketika berada di bawah jajahan Jepang. Sementara So Ji Sub berperan sebagai mantan mafia yang berakhir di Pulau Hashima dan menjadi bagian dari ratusan orang yang menjadi penambang batu bara secara paksa.']</t>
         </is>
       </c>
     </row>
@@ -572,7 +572,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="n">
-        <v>1110</v>
+        <v>1135</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -581,12 +581,12 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>['startup', 'teknologi', 'berita', 'inovasi', 'pengguna', 'indonesia', 'fitur', 'layanan', 'terbaru', 'aplikasi']</t>
+          <t>['startup', 'teknologi', 'berita', 'inovasi', 'pengguna', 'indonesia', 'fitur', 'layanan', 'aplikasi', 'terbaru']</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>['Hari ini DailySocial.id dan MRA (Mugi Rekso Abadi) Group secara resmi mengumumkan kemitraan strategis. Kemitraan ini akan fokus untuk mencapai dua hal: membawa DailySocial.id ke tahap yang lebih tinggi dan memperkuat portfolio MRA Group di industri digital dan gaya hidup. Kerja sama strategis ini secara konkret akan difokuskan ke teknologi media, komunitas, riset, dan inovasi. DailySocial.id sendiri akan tetap fokus di edukasi dan informasi mengenai industri teknologi, inovasi, dan gaya hidup digital. Yang kami hasilkan adalah konten media (artikel, video, infografis) dan \xa0 riset pasar seputar adopsi produk teknologi. Sejak didirikan tahun 2008 silam, DailySocial.id tetap konsisten dalam perjalanan mencapai visi “ menghubungkan masyarakat dengan teknologi “. Kami percaya bahwa teknologi bisa meningkatkan taraf hidup manusia, memajukan peradaban, dan solusi untuk banyak masalah di dunia ini. Dengan adanya kemitraan ini, DailySocial.id bisa memperluas jangkauan dalam melakukan edukasi dan penyebaran informasi mengenai teknologi dan inovasi ke lebih banyak masyarakat Indonesia. We want to go long and far. Sejak awal, \xa0 DailySocial.id selalu fokus ke konten - konten berkualitas dan menjauh dari judul bombastis demi klik. Kenapa? Kami percaya informasi berkualitas dan edukasi bagi para pembaca jauh lebih penting ketimbang \xa0 clicks dan share di jejaring sosial. Kemajuan industri teknologi di Indonesia merupakan prioritas tim, \xa0 bukan \xa0 soal traffic \xa0 atau kuota artikel. Konsistensi visi dan misi ini juga sejalan dengan prinsip bisnis \xa0 DailySocial.id. Dalam beberapa tahun terakhir, tim \xa0 DailySocial.id sudah membangun perusahaan yang sustainable dan juga profitable dari sisi bisnis. Hal ini krusial untuk memberikan kami kekuatan finansial untuk menjaga kualitas dan integritas sebagai media digital. Sebuah keuntungan yang tidak banyak dimiliki pemain lain di Indonesia. Ini merupakan bab baru bagi DailySocial.id. Adalah sebuah kehormatan bisa bekerja sama dengan mitra strategis baru sekelas MRA Group yang bisa membantu \xa0 DailySocial.id mencapai visi dan menjalankan misi sebagai startup media digital. Tentunya hal ini tidak mungkin terjadi tanpa dukungan tim, para pembaca, shareholders, dan \xa0 para rekanan industri. Semuanya demi kemajuan industri teknologi di Indonesia. #StartupIsLife DailySocial.id adalah portal berita startup dan inovasi teknologi. Kamu bisa menjadi member komunitas startup dan inovasi DailySocial.id, mengunduh laporan riset dan statistik seputar teknologi secara cuma-cuma, dan mengikuti berita startup Indonesia dan gadget terbaru.', 'Berbeda dengan layanan Facebook, di Instagram membuat postingan terjadwal belum memungkinkan untuk dilakukan karena memang fiturnya belum tersedia. Tapi itu bukan akhir segalanya, karena ada banyak sekali tools atau aplikasi yang menawarkan fitur tersebut meskipun prosesnya menjadi sedikit lebih panjang. Salah satu aplikasi yang bisa Anda gunakan adalah Hootsuite yang tidak hanya bisa membuat postingan terjadwal ke Instagram tapi juga ke media sosial Twitter dan Facebook. Saya akan coba langsung bagaimana cara kerja Hootsuite ini. Selain Hootsuite, masih ada beberapa aplikasi berbasis mobile yang menawarkan fitur serupa. Saya berikan beberapa opsinya di bawah ini: DailySocial.id adalah portal berita startup dan inovasi teknologi. Kamu bisa menjadi member komunitas startup dan inovasi DailySocial.id, mengunduh laporan riset dan statistik seputar teknologi secara cuma-cuma, dan mengikuti berita startup Indonesia dan gadget terbaru.', 'Setelah memperoleh pembaruan, aplikasi Facebook berbasis Android kini tidak hanya bisa memposting foto dalam format standar dan GIF, tapi juga foto 360 derajat yang makin sering dipilih untuk memotret objek wisata karena tangkapan objeknya yang lebih hidup. Nah, sekarang kita akan mencoba membuat foto 360 derajat menggunakan fitur baru tersebut. Nah, terakhir ada beberapa tips tambahan untuk mendapatkan foto 360 derajat yang oke. Sumber gambar header Pixabay. DailySocial.id adalah portal berita startup dan inovasi teknologi. Kamu bisa menjadi member komunitas startup dan inovasi DailySocial.id, mengunduh laporan riset dan statistik seputar teknologi secara cuma-cuma, dan mengikuti berita startup Indonesia dan gadget terbaru.']</t>
+          <t>['Salah satu fitur unik yang dimiliki semua perangkat smartphone terbaru Xiaomi dengan MIUI 8 adalah Second Space atau yang dapat dikonotasikan sebagai profil kedua tempat di mana Anda bisa memiliki ruang penggunaan yang berbeda. Pembaca yang budiman, itulah tips mengaktifkan fitur Second Space di Xiaomi Redmi 4A. Tapi sebelum berpisah, saya akan berikan beberapa manfaat Second Space untuk Anda. DailySocial.id adalah portal berita startup dan inovasi teknologi. Kamu bisa menjadi member komunitas startup dan inovasi DailySocial.id, mengunduh laporan riset dan statistik seputar teknologi secara cuma-cuma, dan mengikuti berita startup Indonesia dan gadget terbaru.', 'Fitur baru merupakan salah satu pengembang untuk menyenangkan hati penggunanya agar tetap setia menggunakan aplikasinya. Dan biasanya, sebelum merilis sebuah fitur ke publik, pengembang bakal melewati fase uji coba yang lama waktunya tergantung pada umpan balik dan proses perbaikan yang dilakukan. Google termasuk salah satu perusahaan yang menerapkan cara ini. Yang terbaru, mereka sedang menguji fitur baru untuk Chrome versi Android. Fitur baru bernama Breaking News Push disebut sedang dalam tahap pengujian awal. Tersirat dari namanya, ini adalah fitur yang menawarkan notifikasi breaking news ringkas dan pendek. Lebih jauh dijelaskan bahwa fitur ini bakal mengandalkan platform Google Cloud Messaging untuk menerima pemberitahuan instan. Google Cloud Messaging sendiri sebenarnya adalah platform yang diciptakan untuk memudahkan pengembang mengirim informasi ke aplikasi android. Secara teknis, ini bukan fitur untuk mereka, tapi Google tampaknya ingin mencobanya sendiri untuk merealisasikan fitur breaking news di Chrome. Namun jika berkaca pada rencana garis besarnya, saya sedikit banyak sudah memperoleh gambaran akan seperti apa implementasi dari ide ini. Menurut saya, notifikasi ini bakal menghantarkan berita-berita terbaru terkurasi yang dikutip dari penerbit - penerbit pilihan. Jika selama ini kebanyakan konten semacam ini disuguhkan di dalam browser, Google tampaknya ingin mencoba sesuatu yang berbeda; melalui push notifications yang bagi kebanyakan orang justru dianggap mengganggu kenyamanan bergadget ria. Untuk mengatasinya, Google punya alternatif cara dengan mencoba menghantarkan pilihan berita yang sesuai dengan minat dan preferensi masing-masing pengguna. Jika demikian, bukan tidak mungkin suatu saat teknologi AI bakal dilibatkan di sini. Sumber berita AndroidPolice dan ChromeStory. DailySocial.id adalah portal berita startup dan inovasi teknologi. Kamu bisa menjadi member komunitas startup dan inovasi DailySocial.id, mengunduh laporan riset dan statistik seputar teknologi secara cuma-cuma, dan mengikuti berita startup Indonesia dan gadget terbaru.', 'Pada bulan April tahun ini, Instagram mengumumkan bahwa mereka memiliki lebih dari 700 juta pengguna aktif di jejaring sosialnya. Kini, seperti dilansir CNBC, platform berbagi gambar dan video itu kembali mengumumkan pencapaian baru sebanyak 100 juta pengguna tambahan sehingga total ada 800 juta pengguna aktif yang mengakses platformnya setiap bulan, dan ada 500 juta pengguna yang aktif setiap harinya. Fitur barunya, Stories nampaknya menjadi aktor di balik kesuksesan ini. Sejak Stories diluncurkan setahun lalu, menurut TheVerge, jumlah pengguna Instagram tercatat meningkat sebesar 160 persen. Video juga menjadi salah satu indikator yang tak kalah penting. Perusahaan tersebut mengatakan bahwa pengguna memproduksi video empat kali lebih banyak dibandingkan tahun lalu. Akibatnya, waktu yang dihabiskan untuk menonton video di platform itu juga naik lebih dari 80 persen dari tahun ke tahun. Peningkatan dari berbagai sisi tersebut secara otomatis turut berdampak pada angka pengiklan di Instagram. Per September 2017, Instagram mempunyai total 2 juta pengiklan yang sebagian besar datang dari bisnis kecil menengah. Jika dibandingkan, angka ini dua kali lipat dari statistik yang didapat pada bulan Maret lalu. Facebook membeli Instagram pada awal tahun 2012 seharga $1 miliar secara tunai. Di atas kertas, nominal ini tentu tidaklah sedikit, tapi jelas sekali bahwa jejaring sosial raksasa itu tahu investasinya tak akan sia-sia. Manuver investasi suskes lainnya adalah pembelian \xa0 WhatsApp seharga $19 miliar dan kini menjadi salah satu platform aplikasi pesan paling ngetop di dunia. Sumber berita NCBC dan gambar header Pixabay. DailySocial.id adalah portal berita startup dan inovasi teknologi. Kamu bisa menjadi member komunitas startup dan inovasi DailySocial.id, mengunduh laporan riset dan statistik seputar teknologi secara cuma-cuma, dan mengikuti berita startup Indonesia dan gadget terbaru.']</t>
         </is>
       </c>
     </row>
@@ -598,21 +598,21 @@
         <v>4</v>
       </c>
       <c r="C7" t="n">
-        <v>587</v>
+        <v>833</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4_trump_negara_presiden_israel</t>
+          <t>4_makanan_tubuh_indonesia_orang</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>['trump', 'negara', 'presiden', 'israel', 'orang', 'amerika', 'serangan', 'isis', 'palestina', 'militer']</t>
+          <t>['makanan', 'tubuh', 'indonesia', 'orang', 'memiliki', 'makan', 'air', 'kanker', 'penyakit', 'kulit']</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>['Jakarta, CNN Indonesia - - Presiden Amerika Serikat Donald Trump dan Presiden Rusia Vladimir Putin berdiskusi mengenai solusi konflik Suriah hingga krisis nuklir Korea Utara melalui telepon pada Selasa (2 / 5) waktu setempat. Perbincangan kedua pemimpin ini merupakan yang pertama setelah hubungan Washington dan Moskow sempat merenggang akibat serangan udara AS ke Suriah, sekutu dekat Rusia, pada awal April lalu. Seorang pejabat senior AS \xa0 mengaku, Putin lah yang pertama kali meminta untuk menghubungi Trump. Dalam percakapan, Trump dan Putin dikabarkan sepakat meningkatkan dialog untuk mencari solusi memperkuat dan menjaga stabilitas gencatan senjata di Suriah. Keduanya juga turut membahas kemungkinan membentuk zona aman bagi warga sipil yang terdampak perang di negara Timur Tengah itu. Menurut Gedung Putih, kedua pemimpin sepakat bahwa " semua pihak wajib melakukan apa yang mereka bisa untuk mengakhiri kekerasan " di negara itu. " Percakapan mereka sangat baik, membahas zona aman atau de - eskalasi guna mencapai perdamaian kemanusiaan yang abadi dan berbagai persoalan lainnya, " bunyi pernyataan Gedung Putih pada Rabu (3 / 5). Kantor presiden AS itu menyebutkan, Trump juga menyatakan akan mengirimkan perwakilan negaranya sebagai pengamat \xa0 dalam perundingan gencatan senjata antara rezim Suriah dan kelompok oposisi di Astana, Kazakhstan pada Rabu dan Kamis pekan ini. Hal ini dinilai menggambarkan keseriusan AS untuk berkontribusi dalam upaya perdamaian Suriah. " Tujuannya untuk mendorong realisasi solusi damai bagi Suriah, " ucap kantor tersebut. Selain itu, Kremlin menyatakan, perbincangan Putin dan Trump turut membahas " solusi terbaik mengatasi situasi berbahaya di Korea Utara . " Korut terus menjadi sorotan setelah pada awal tahun baru lalu, pemimpin tertinggi mereka, Kim Jong - un, memerintahkan penguatan program rudal balistik antarbenua (ICBM) negaranya. Sepanjang tahun ini, Pyongyang tercatat sudah meluncurkan sejumlah uji coba rudal, dua di antaranya mencapai perairan di dekat wilayah Jepang. Dengan ambisi rudal nuklirnya, negara paling terisolasi ini menjadi salah satu tantangan utama global. Putin dan Trump turut mendiskusikan cara menyelesaikan krisis yang telah menimbulkan ketegangan di seluruh kawasan Asia Pasifik ini. " Situasi sangat berbahaya di Semenanjung Korea dibahas secara rinci. Presiden Putin menyerukan agar seluruh pihak menahan diri dan mengurangi ketegangan, " kata Kremlin seperti dilansir dari Reuters. Dalam kesempatan itu, kedua presiden juga turut mendiskusikan strategi memerangi terorisme dan kelompok militan di Timur Tengah, khususnya ISIS. Terorisme masih menjadi fokus utama keamanan bagi kedua negara. Putin dan Trump juga membahas rencana pertemuan tatap muka pertama mereka yang diagendakan berlangsung di sela-sela pertemuan KTT G - 20 do Hamburg pada 7 - 8 Juli mendatang.', 'Washington (ANTARA News) - Calon presiden dari Partai Republik Donald Trump pada Minggu (25 / 9) memberitahu Perdana Menteri Israel Benjamin Netanyahu bahwa jika dia terpilih maka Amerika Serikat akan mengakui Yerusalem sebagai ibu kota Israel menurut tim kampanyenya. Dalam pertemuan satu jam lebih dengan Netanyahu di Trump Tower, New York, Trump mengatakan kepada Netanyahu bahwa di bawah pemerintahannya Amerika Serikat akan " mengakui Yerusalem sebagai ibu kota tak terbagi bagi Negara Israel . " Israel menyebut Yerusalem sebagai ibu kotanya dan beberapa negara termasuk Amerika Serikat menerimanya, namun kebanyakan negara menempatkan kedutaan besarnya di Tel Aviv. Warga Palestina menginginkan Yerusalem Timur, yang direbut Israel dalam perang tahun 1967, sebagai ibu kota negara yang mereka bentuk di samping Israel di Tepi Barat dan Jalur Gaza. Dalam pertemuan tertutup dengan Netanyahu, menurut tim kampanyenya Trump sepakat dengan Netanyahu bahwa perdamaian di Timur Tengah hanya bisa dicapai ketika " warga Palestina meninggalkan kebencian dan kekerasan dan menerima Israel sebagai Negara Yahudi . " Menurut notulensi pertemuan dari tim kampanye Trump, keduanya juga mendiskusikan " panjang " pagar batas Israel, mengutip Trump mengacu pada kebijakan imigran kontroversial dia yang meliputi pembangunan dinding di perbatasan Amerika Serikat dan Meksiko dan sementara melarang Muslim memasuki negaranya. Diskusi keduanya juga meliputi masalah-masalah regional lain seperti perang melawan ISIS, bantuan militer Amerika Serikat untuk Israel yang disebut " investasi terbaik " dan kesepakatan nuklir Iran, yang dikritik kedua pihak, demikian menurut warta kantor berita Reuters.', 'AMERIKA– Majelis Umum PBB sudah melakukan penghitungan suara atas resolusi yang mendesak Amerika Serikat harus menarik keputusan yang menyatakan Yerusalem sebagai ibu kota Israel. Dalam pemungutan suara Kamis (21 / 12) waktu New York, sebanyak 128 negara mendukung resolusi, sembilan menentang, dan 35 negara memilih untuk abstain. Sehari sebelumnya, Presiden Donald Trump mengeluarkan ancaman akan memutus bantuan keuangan bagi negara-negara yang menentang keputusannya dalam menetapkan Yerusalem sebagai ibu kota Israel. Sebelum pemungutan suara dimulai, Menteri Luar Negeri Palestina, Riad al - Malki, mendesak ahgar negara-negara anggota PBB menolak ‘ pemerasan dan intimidasi’. Sementara Perdana Menteri Israel, Benjamin Netanyahu mengatakan akan menolak sama sekali hasil yang menurutnya sudah diantisipasi dan menyebut PBB sebagai ‘ rumah kebohongan’. _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ Sekilas komposisi suara -. Sembilan negara yang menolak adalah Amerika Serikat, Israel, Guatemala, Honduras, Kepulauan Marshall, Mikronesia, Nauru, Palau, dan Togo -. Yang abstain antara lain Kanada dan Meksiko -. Indonesia termasuk dalam 128 negara yang mendukung resolusi, bersama empat negara anggota tetap Dewan Keamanan: Cina, Prancis, Rusia, dan Inggris. -. Sebanyak 21 negara tidak hadir untuk memberikan suara _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ _ \n Indonesia merupakan salah satu negara yang mendukung resolusi PBB tersebut. “ Indonesia tetap konsisten sejak dulu dalam mendukung kepentingan rakyat Palestina, ” kata Juru bicara Istana Kepresidenan, Johan Budi, di Jakarta kepada BBC Indonesia, sebelum pemungutan suara. Ketika masih di tingkat Dewan Keamanan PBB, Amerika Serikat sudah memveto rancangan resolusi yang menolak keputusan Presiden Donald Trump untuk mengakui Yerusalem sebagai ibu kota Israel. Dalam sidang DK PBB awal pekan ini, Duta Besar AS untuk PBB, Nikki Haley, mengatakan bahwa draf resolusi tersebut merupakan ‘ penghinaan’. Awal bulan ini Trump menyatakan Yerusalem adalah ibu kota Israel, walau sejak awal sudah dikecam dunia internasional dan belakangan memicu aksi unjuk rasa di sejumlah tempat. Hari Rabu (21 / 12), Presiden Trump mengeluarkan ancaman atas negara-negara yang akan menentang mereka saat penghitungan suara di Majelis Umum PBB ini. “ Mereka mengambil jutaan dolar dan bahkan miliaran dolar dan mereka memberi suara yang menentang kita, ” katanya kepada para wartawan di Gedung Putih, Rabu (20 / 12). “ Biarkan mereka bersuara menentang kita. Kita akan menghemat banyak. Kita tidak perduli. Sementara itu Duta Besar AS untuk PBB, Nikki Haley, memperingatkan negara anggota PBB bahwa Presiden Trump memintanya untuk melaporkan ‘ siapa yang menentang kita’ pada pemungutan suara di Majelis Umum PBB. Status Yerusalem merupakan masalah utama dalam konflik Israel - Palestina dengan Palestina mengklaim Yerusalem Timur sebagai ibu kota dari negara masa depan mereka. Penetapan Trump bahwa Yerusalem merupakan ibu kota Israel dianggap berbagai pihak akan semakin menghambat proses perundingan damai, yang dalam beberapa waktu belakangan ini memang sudah terhenti. (BBC)']</t>
+          <t>['Jakarta, CNN Indonesia - - Saat musim hujan seperti sekarang ini, tubuh lebih rentan terkena flu. Beragam suplemen dan obat pun dikonsumsi demi tubuh yang bebas dari flu. Padahal, obat terbaik saat flu hanyalah istirahat. Namun saat flu, tubuh harus terhidrasi dan juga memerlukan nutrisi. Makanan yang bernutrisi akan membantu tubuh mengurangi rasa tidak nyaman akibat flu. Mengutip travelandleisure, dua ahli gizi merekomendasikan makanan atau minuman yang cocok dikonsumsi saat terserang flu. Makanan ini akan bermanfaat untuk meningkatkan kekebalan tubuh. 1. Minuman Elektrolit Hal terpenting saat terkena flu adalah menjaga tubuh agar tetap terhidrasi dengan baik, apalagi jika flu disertai dengan demam. Ahli gizi Jessica Crandal, yang berbasis di Denver menyarankan untuk banyak mengonsumsi air putih. Selain itu, tambahan minuman elektrolit atau air kelapa juga membantu tubuh mendapatkan sodium dan potassium. Minuman elektrolit yang memiliki aroma mungkin akan lebih menarik seseoarang untuk meningkatkan konsumsi air. Minuman elektrolit juga menjadi pengganti makanan yang membantu tubuh mendapatkan kalori yang dibutuhkan. 2. Teh Hijau Seorang ahli gizi Rena Zelig, RDN, mengatakan flu akan mengganggu saluran pernapasan bagian atas. Minuman hangat atau panas dapat membantu melegakan saluran pernapasan. Zelig merekomendasikan untuk mengonsumsi teh hijau karena kandungan antioksidan lebih tinggi. Tambahkan sedikit madu pada teh hijau, yang bermanfaat untuk menenangkan sakit tenggorokan dan meredakan batuk. 3. Sup Ayam Rasa asin dari kaldu ayam bisa membantu tubuh agar tetap terhidrasi dan juga mengganti sodium yang hilang. Sayuran yang ada pada sup bisa menjadi sumber vitamin dan mineral. Ayam menyediakan protein yang bermanfaat untuk penyembuhan dan bisa memberikan tenaga untuk tubuh. Para ilmuwan mengatakan aroma dari sup bisa melonggarkan hidung tersumbat dari lendir akibat flu. Sup ayam juga membantu sel-sel darah putih melawan infeksi sehingga bekerja lebih efisien. 4. Kacang - kacangan Protein juga bisa didapat dengan mengonsumsi kacang-kacangan seperti kacang polong. Kacang - kacangan ini bisa dinikmati ketika diolah menjadi sup. 5. Buah dan Sayur Untuk melindungi tubuh dari penyakit kronis, sangat diperlukan makanan yang mengandung antioksidan. Zelig mengatakan antioksidan berperan dalam menjaga kesehatan dan meningkatkan sistem kekebalan tubuh. Ia merekomendasikan untuk mengonsumsi buah atau sayur yang bewarna cerah seperti paprika, jeruk, dan buah beri. 6. Jus Jeruk Jus jeruk menjadi sumber vitamin C yang baik bagi tubuh. Beberapa penelitian mengatakan mengonsumsi jus jeruk dapat mengurangi pilek dan flu. Namun tubuh tidak bisa menyerap vitamin C secara berlebihan. Untuk itu Crandall menyarankan untuk mencampur empat ons jus jeruk dengan 16 - 20 ons air. Dengan begitu tubuh akan mendapatkan vitamin C tanpa kandungan gula dan kalori yang berlebihan.', 'Buat sebagian orang, berolahraga dianggap cukup melelahkan, apalagi jika kamu juga berusaha untuk melakukan diet dan menurunkan berat badan. Namun, sadar atau enggak, untuk hidup sehat, kamu enggak perlu melakukan diet ketat atau olahraga berat setiap hari. Sebab, kamu cukup melakukan lima hal sederhana berikut ini, agar kamu mendapatkan tubuh yang sehat. Apa saja? Berikut rangkuman kumparan (kumparan.com) seperti yang dikutip dari Her World. 1. Buat makan siang sendiri Ini merupakan salah satu hal sederhana yang bisa kamu lakukan saat harus mengerjakan beberapa tugas menumpuk di kantor. Bangun lebih pagi dan memasukkan beberapa bahan makanan tertentu bisa membuat kamu lebih sehat. Hal ini juga bisa kamu lakukan saat makan malam. 2. Minum air yang cukup Minum air penting untuk menjaga cairan yang ada pada tubuh. Selain itu, meminum air yang cukup juga akan membantu kamu untuk mengurangi rasa lapar sehingga membuat kamu enggak mengonsumsi terlalu banyak makanan. Hal ini ampuh untuk menurunkan berat badan kamu, lho. 3. Jangan makan sampai kenyang Enggak semua makanan yang ada di atas piring makan siang kamu harus dilahap habis. Namun, hal ini bukan berarti kamu harus membuangnya, tapi kamu harus mengurangi porsi makanan sebelum menyantapnya. Otak membutuhkan waktu sekitar 20 menit untuk mendefinisikan bahwa tubuh kita sudah kenyang atau belum. Itu sebabnya, usahakan untuk mengendalikan jumlah makanan yang kamu makan. 4. Tidur yang cukup Ini merupakan salah satu cara paling mudah dan sempurna untuk kamu yang ingin hidup sehat. Tubuh membutuhkan waktu tidur sekitar 7 hingga 9 jam pada malam hari. Karenanya, singkirkan semua gangguan yang bisa mengganggu tidur kamu saat berada di tempat tidur ya. 5. Sayuran dan buah beku Sayur dan buah segar enggak bisa bertahan terlalu lama saat kamu membawanya pulang. Di sisi lain, kegiatan dan aktivitas kamu yang padat membuat kamu enggak bisa selalu belanja ke pasar atau supermarket untuk membeli sayur dan buah yang segar. Karenanya, coba ganti dengan sayur dan buah beku yang memiliki kandungan antioksidan dan nutrisi yang hampir sama dengan sayur dan buah yang segar.', "Ungkapan' you are what you eat' atau yang artinya kamu adalah apa yang kamu makan memang benar. Namun, apa yang terjadi pada tubuh nyatanya tak hanya dipengaruhi oleh makanan yang dimakan saja, melainkan juga turut dipengaruhi dari kebiasaan makan seseorang. Dilansir Times of India, kegiatan sesudah makan juga menjadi hal yang harus diperhatikan jika ingin memiliki tubuh yang sehat. Membiarkan tubuh mencerna makanan setelah makan atau tak langsung tidur adalah contoh perilaku yang seharusnya diterapkan sesaat setelah kegiatan bersantap usai. Selain dua contoh itu, masih ada beberapa poin penting lainnya yang perlu diketahui masyarakat mengenai sikap yang dilarang setelah makan. Bagi yang ingin tahu selengkapnya, yuk simak ulasan di bawah ini: 1. Tidak Merokok Hal pertama yang harus dihindari adalah merokok. Sejatinya, merokok merupakan kebiasaan buruk yang patut dijauhi. Kebiasaan ini menjadi 10 kali lebih berbahaya jika dilakukan sesaat setelah makan karena setidaknya rokok mengandung 60 zat karsinogen yang menyebabkan penyakit kanker. Karenanya, hindari merokok setelah makan. 2. Tidak Bergegas Mandi Tubuh membutuhkan energi untuk mencerna semua makanan yang masuk. Jika, kamu memilih mandi setelah makan maka, energi yang seharusnya dibutuhkan oleh tubuh untuk mencerna makanan mendadak berkurang akibat aliran pembuluh darah terhalau akibat dampak air dingin yang mengenai kulit. Berikan jeda sekitar 30 menit sampai sistem metabolisme tubuh mencerna semua makanan yang masuk ke dalam tubuh. 3. Tidak Minum Teh atau Kopi Ada waktu terbaik untuk menikmati kedua minuman ini. Namun, bukan setelah makan. Menurut sebuah penelitian, kopi dan teh baru bisa dinikmati setelah semua makanan berhasil dicerna oleh tubuh. Dan proses pencernaan ini membutuhkan waktu hingga 60 menit. Artinya, kamu baru bisa meminum secangkir kopi atau teh setelah satu jam sehabis makan. 4. Tidak Langsung Makan Buah Beberapa orang mungkin mengatakan bahwa buah bisa dikonsumsi kapan saja, termasuk setelah makan. Namun, rupanya kebeneran ini perlu ditinjau kembali karena pasalnya mengkonsumsi buah setelah makan hanya akan menyebabkan pencernaan buah di dalam usus tidak berjalan lancar. Hal ini juga mengacaukan proses pencernaan makanan sebelumnya. 5. Tidak Berjalan Berjalan kaki setelah makan dianggap menjadi cara terbaik dalam membantu melancarkan proses pencernaan secara cepat. Padahal, hal ini tidak diperbolehkan karena makanan perlu dicerna terlebih dahulu sampai tubuh siap untuk berjalan kembali. Berikan waktu sekitar 30 menit sampai semua makanan yang masuk ke dalam tubuh dicerna secara sempurna. 6. Tidak Langsung Tidur Tak boleh langsung berbaring, tidur setelah makan hanya akan membuat proses pencernaan terganggu. Karena makanan yang seharusnya bisa dialiri sempurna untuk sampai ke usus akan berpindah haluan ke arah yang berlawanan. Oleh sebab itu, biarkan tubuh mencerna makanan terlebih dahulu dengan melakukan kegiatan lain, misalnya menonton tv atau mendengarkan radio. 7. Melonggarkan Ikat Pinggang Sebenarnya hal ini tidak dilarang, namun melonggarkan ikat pinggang setelah makan menjadi sebuah alarm yang menandakan jika kamu sudah terlalu banyak makan. Rasa kenyang berlebihan tentu bukan menjadi tanda yang baik, melainkan sebuah tanda peringatan agar kamu bisa membatasi porsi makan yang seharusnya."]</t>
         </is>
       </c>
     </row>
@@ -624,21 +624,21 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>395</v>
+        <v>552</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>5_indonesia_wisata_budaya_makanan</t>
+          <t>5_trump_negara_presiden_israel</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>['indonesia', 'wisata', 'budaya', 'makanan', 'pariwisata', 'festival', 'kopi', 'kota', 'pulau', 'wisatawan']</t>
+          <t>['trump', 'negara', 'presiden', 'israel', 'orang', 'serangan', 'amerika', 'militer', 'palestina', 'isis']</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>['Jakarta, CNN Indonesia - - Seni budaya Indonesia bakal mejeng di setiap sudut Belgia, negara ibukota Uni Eropa. Indonesia didapuk menjadi tamu kehormatan yang secara otomatis juga menjadi negara tema untuk ajang festival seni budaya bergengsi di Eropa, Europalia 2017. Festival itu merupakan ajang budaya terbesar di Eropa yang diselenggarakan Kerajaan Belgia setiap dua tahun sekali sejak 1959. Setiap penyelenggaraannya, Belgia menunjuk satu negara tamu untuk memamerkan seni dan budaya di 36 kota dan delapan negara di Eropa selama hampir empat bulan. Tahun ini, giliran Indonesia yang bakal unjuk gigi di negeri barat itu, di bawah arahan Kementerian Pendidikan dan Kebudayaan. Sebelumnya baru ada tiga negara Asia yang pernah menjadi negara tamu di Europalia, yakni Jepang (1989), China (2009), dan India (2013). " Ini sangat penting bagi kami unuk mengetahui apa yang terjadi di Indonesia sejak dahulu kala sampai saat ini. Karena kami tidak punya ritual dan tradisi leluhur seperti ini, " kata perwakilan Pemerintah Belgia dan Europalia, Drik Vermaelen saat temu media di Museum Nasional, Jakarta, Senin (11 / 7). Bertajuk ‘ Rampai Indonesia di Eropa,’ Indonesia bakal memamerkan lebih dari 400 benda-benda berharga dari zaman purbakala hingga era modern. Benda bersejarah yang datang dari berbagai daerah di Indonesia itu dibagi dalam dua kategori pameran: Ancestor dan Archipel. Pemilihannya dilakukan oleh kurator asal Belgia dan Indonesia. Pameran Ancestor bakal menceritakan aneka ragam budaya Indonesia menghargai leluhur. Dalam kategori pameran ini, sebanyak 167 benda peninggalan leluhur akan dibawa ke Belgia. Benda - benda itu akan memberikan gambaran tradisi Indonesia mulai dari kirab hingga mudik. Untuk pameran Archipel, Indonesia akan menunjukkan budaya maritim yang sudah berkembang sejak dahulu kala, mulai teknologi perkapalan, pengetahuan navigasi dan beragam tradisi. Di kategori ini pemerintah membawa 250 benda yang berkaitan dengan budaya maritim. Untuk memperkuat budaya, sebuah replika kapal Bugis saat ini tengah dibuat di Bulukumba untuk bisa dipamerkan di Belgia, Oktober mendatang. " Tujuannya menunjukkan sejarah maritim dan budaya Indonesia dan seiring dengan visi Indonesia sebagai poros maritim dunia, " kata Anggota Tim Ahli Pameran Archipel, Singgih Tri Sulistyono. Mayoritas benda-benda itu merupakan koleksi dari Museum Nasional. Sebagiannya lagi dikirim dari museum lokal di berbagai daerah dan beberapa merupakan koleksi pribadi. Ratusan benda yang akan dikirim itu memiliki ukuran dan berat yang bermacam-macam, bahkan ada yang mencapai satu ton. Artefak itu juga terbuat dari berbagai bahan seperti kayu, batu, tengkorak, perunggu, hingga emas. Koleksi tersebut juga dibagi berdasarkan periode terbentuknya, mulai periode kuno (3000 sebelum masehi), periode pra modern (abad 1 - 15), periode awal modern (abad 7 - 18), hingga periode modern (abad 19 sampai sekarang). Selain dua pameran utama, Europalia bertema Indonesia ini juga melibatkan lebih dari 400 pekerja seni dalam bidang tari, pertunjukkan, musik, instalasi, film. Sebanyak 226 karya dan juga program akan menghibur penonton yang diperkiran bakal mencapai lebih dari 1,5 juta orang. Kebudayaan Indonesia akan mulai dipamerkan pada 10 Oktober 2017 hingga 21 Januari 2018.', 'Jakarta, CNN Indonesia - - Festival Seni Budaya Europalia dibuka hari ini, Selasa (10 / 10) di Brussel, Belgia. Terdapat sekitar 316 seniman yang terlibat, juga ratusan barang seni serta benda bersejarah yang dipamerkan. Produk sastra dan seni budaya lain, seperti pertunjukan, film, sampai pameran destinasi wisata pun termasuk ke dalam agenda festival besar itu. Acaranya sendiri digelar selama empat bulan, sejak bulan ini hingga Januari 2018. Tak hanya di satu tempat, seni - seni yang ada juga akan berkeliling ke tujuh negara. Menurut keterangan pers yang diterima CNNIndonesia.com, produk seni Indonesia juga bisa dinikmati di Belgia, Inggris, Perancis, Polandia, Jerman, Belanda, dan Austria. Festival Seni Budaya Europalia diselenggarakan setiap dua tahun sekali. Tahun ini, Wakil Presiden Jusuf Kalla dan Menteri Koordinator Bidang Pembangunan Manusia dan Kebudayaan Puan Maharani hadir membukanya. Sehari sebelumnya, mereka bertemu Wakil Presiden Uni Eropa Andrus Ansip membahas potensi kerja sama Eropa dengan Indonesia. Pertemuan berlangsung selama satu jam, Senin (9 / 10). Dari pertemuan itu, disimpulkan bahwa kerja sama ekonomi antara Eropa dengan Indonesia bisa terjalin melalui Europalia. Seperti yang disebutkan Puan, festival itu bisa menjadi pintu gerbang bagi peluang kerja sama yang lebih besar bagi negara-negara itu. Puan mengatakan, Indonesia bertaruh banyak demi penyelenggaraan festival itu. Indonesia sampai mengeluarkan biaya sekitar Rp 160 miliar. Namun itu dilakukan, katanya, karena reputasi festival yang sudah sangat kuat dan daya tariknya di kalangan masyarakat Eropa. Bukan hanya mempromosikan seni dan budaya, Europalia juga menjadi ajang promosi wisata Indonesia. Lewat festival itu, jadi banyak warga asing yang mengenal Indonesia, sehingga semakin tinggi pula kedatangan turis mancanegara yang ingin menikmati keindahannya. “ Festival Seni Budaya Europalia diharapkan menjadi momentum bagi Indonesia untuk menunjukkan kekayaan seni dan budayanya, agar semakin dikenal oleh dunia internasional, khususnya masyarakat Eropa, ” ujar Puan dalam keterangan resminya.', 'London (ANTARA News) - Pertunjukkan galeman yang dibawakan warga Rusia dan tarian Nusantara dari Tim Kesenian KBRI Moskow memukai warga Suzdal dalam acara Hari Budaya Indonesia di Museum Vladimir &amp; Suzdal, kota Suzdal, salah satu kota Golden Ring Rusia, sekitar 270 km dari Moskow, akhir pekan. Pergelaran   dibawakan pemain gamelan Dadali dan penari " Kirana Nusantara Dance " di bawah bimbingan Tri Koyo, pelatih gamelan dan Elisabeth Nur Nilasari, pelatih tari KBRI Moskow, demikian Sekretaris Pertama Fungsi Pensosbud KBRI Moskow, Enjay Diana kepada Antara London, Selasa. Dikatakannya sebagian besar anggota tim kesenian tersebut merupakan warga Rusia pecinta budaya Indonesia yang menunjukkan kepiawaiannya dalam bermain gamelan dan menari tarian Indonesia. Direktur Jenderal Museum Vladimir &amp; Suzdal, Igor Konyshev mengatakan kehadiran   tim kesenian KBRI Moskow dipimpin Dubes M. Wahid Supriyadi memberi kesan    mendalam bagi masyarakat Suzdal yang mendapat kesempatan   langka menikmati penampilan kesenian Indonesia yang beraneka ragam dan unik. Terlebih lagi, pergelaran Hari Budaya Indonesia yang diadakan pada hari Sabtu (2 / 12) ini merupakan pertama kali diadakan di kota Suzdal, kota Kabupaten mampu menarik lebih dari 1 juta wisatawan baik dalam maupun luar negeri, kata Igor Konyshev. Dubes Indonesia untuk Federasi Rusia merangkap Republik Belarus, M. Wahid Supriyadi mengatakan penyelenggaraan Hari Budaya Indonesia di berbagai daerah di Rusia, termasuk di kota Suzdal merupakan upaya KBRI Moskow untuk memperkenalkan Indonesia kepada masyarakat Rusia. Kedua negara telah memiliki hubungan baik di berbagai bidang kerja sama, mulai dari politik, ekonomi hingga sosial budaya, ujarnya. Menurut Dubes Wahid Supriyadi, pemahaman yang semakin baik mengenai Indonesia oleh masyarakat Rusia turut mendorong terjadinya peningkatan people to people contact. Hal ini antara lain terlihat dari semakin meningkatnya jumlah wisatawan Rusia ke Indonesia yang signifikan. Hingga September lalu wistawan Rusia ke Indonesia mencapai lebih dari 81 ribu, atau naik 52% dibandingkan periode yang sama tahun 2016 dan peningkatan tertinggi dibanding pertumbuhan jumlah wisatawan asing dari negara lain ke Indonesia. Tercatat peningkatan volume perdagangan bilateral Indonesia - Rusia untuk periode Januari - September 2017 yang mencapai USD 1,8 milyar atau naik 22% dibandingkan periode yang sama tahun lalu sebesar USD 1,5 milyar, serta frekuensi saling kunjung antar pejabat tinggi kedua negara, kata Dubes Wahid Supriyadi. Penampilan beberapa komposisi klasik Jawa oleh gamelan dan berbagai tarian Indonesia dari Sumatera Utara, Sumatera Barat, Jawa Barat, Jawa Tengah dan Sulawesi Selatan selama dua jam ditutup dengan tarian Gemu Famire. Para pengunjung yang tidak beranjak dari tempat duduknya sejak awal pertunjukan, termasuk anak-anak dengan sigap langsung bergabung ikut menari di panggung di akhir pertunjukan dan tidak ketinggalan   Dubes Wahid Supriyadi. Rangkaian Hari Budaya Indonesia di kota Suzdal diawali dengan workshop tarian tradisional Indonesia dan gamelan oleh Darmawan Suparno, Koordinator Fungsi Pensosbud KBRI Moskow. Workshop diikuti   siswa-siswi dari sekolah musik &amp; tari di kota Suzdal. Para peserta dengan antusias mengikuti penjelasan maupun instruksi yang diberikan mengenai cara memainkan berbagai instrumen gamelan maupun dalam memperagakan tarian, seperti Randai dari Sumatera Barat. Seusai workshop pun siswa-siswi enggan meninggalkan ruangan dan asyik berdiskusi sambil mempraktekkan kembali gerakan Tari Randai yang mereka pelajari, ujar Elisabeth Nur Nilasari, pelatih tari KBRI Moskow. Kota Suzdal merupakan salah satu kota wisata dan bersejarah di Rusia yang termasuk dalam 8 kota Golden Ring Rusia. Suzdal dan Kabupaten Samosir sedang merintis kerja sama Kota Kembar (Sister City). Pada bulan Agustus lalu pada   acara Festival Indonesia kedua di Moskow, Bupati Samosir   mengadakan pembicaraan dengan Walikota Suzdal.']</t>
+          <t>['Suara.com -. Pemerintah Israel berharap, negara-negara lain akan mengikuti tindakan negeri ‘ Pakde Sam’ mengakui kota suci ini sebagai ibu kota Israel. Dia menambahkan, banyak negara juga akan memindahkan kantor kedutaan besar mereka dari Tel Aviv ke Yerusalem ketika Washington memindahkan pusat misi diplomasi mereka ke kota tersebut. “ Beberapa negara mungkin malah memindahkan kedutaan besar mereka ke Yerusalem sebelum AS, ” lanjut juru bicara tersebut. “ Israel menyerukan kepada negara lain untuk mengikuti langkah AS . ” Juru bicara Israel ini juga mengungkap, mereka sedang mengontak beberapa negara untuk mengikuti AS mengakui Yerusalem, meski dia menolak untuk menyebut nama-nama negara tersebut. Pada Rabu (6 / 12) pekan lalu, Presiden Donald Trump secara resmi mengakui Yerusalem sebagai ibu kota Israel, dan memulai persiapan untuk memindahkan kedutaan besarnya dari Tel Aviv ke Yerusalem. Deklarasi itu membalikkan kebijakan AS yang selama berpuluh tahun berusaha netral soal kota suci tersebut. Aksi AS ini memicu protes luas di daerah Palestina dan beberapa negara lain, termasuk kecaman dari negara-negara Arab dan Muslim sedunia. Sekutu - sekutu Washington dari Eropa juga mengkritik langkah Trump, memperingatkan kalau keputusan ini bisa memperburuk hubungan Palestina dengan Israel dan memicu kekisruhan di wilayah tersebut. Kanselir Jerman Angela Markel berkata, “ Pemerintah Jerman tidak mendukung keputusan ini, karena status Yerusalem harus diputuskan dalam bingkai pencarian solusi kedua negara, ” menurut unggahan Twitter juru bicaranya. Presiden Prancis Emmanuel Macron menyebut aksi AS sebagai “ keputusan AS yang patut disesalkan dan tidak mendapat dukungan Prancis, juga menyalahi hukum internasional dan resolusi DK PBB . ” Menteri Luar Negeri Inggris Boris Johnson berkata keputusan AS ini akan mengganggu usaha mewujudkan perdamaian di Timur Tengah. Yerusalem tetap berada di pusat konflik Israel - Palestina, dengan Palestina berharap Yerusalem Timur – sekarang diduduki oleh Israel – menjadi ibu kota negara Palestina kelak. Untuk diketahui, selain Israel sendiri, hanya sedikit negara yang mengakui Yerusalem sebagai ibu kota mereka. Negara - negara yang mengakui Yerusalem ibu kota Israel adalah AS, Taiwan, Vanuatu, dan Republik Ceko. Hal yang mustahil Uri Savir, mantan jenderal manajer di kementerian luar negeri Israel, mengatakan pengakuan negara-negara lain atas Yerusalem sebagai ibu kota Israel mengikuti AS sangat kecil kemungkinanannya. Dia justru berkata, tindakan Trump malah melemahkan posisi Israel soal Yerusalem. “ Keputusan ini menggiring konsensus internasional untuk mencari pemecahan yang melibatkan kedua negara, ” lanjut dia. Menurut Savir lagi, keputusan AS ini juga tidak akan mendapatkan dukungan internasional. “ Sebaliknya, AS kini kehilangan perannya sebagai mediator perdamaian, ” ujar Savir. “ AS tidak lagi dipandang sebagai mediator yang adil . ” Diplomat Israel ini juga berujar tidak ada yang berubah di lapangan setelah pengakuan AS terhadap Yerusalem sebagai ibu kota Israel. “ Masih dibutuhkan negosiasi untuk mencapai kesepakatan soal status final kota ini, ” lanjut Savir. “ Kita harus menemukan ide baru yang kreatif, entah itu meyakinkan Trump untuk memberikan proposal baru atau membawa pihak lain seperti EU untuk turut andil dalam proses negosiasi, ” kata dia.', 'Presiden Amerika Serikat Donald Trump secara resmi mengakui Yerusalem sebagai ibu kota Israel. Hal itu memicu kecaman dari seluruh negara di dunia termasuk Indonesia. Ketua Komisi 1 DPR RI Abdul Kharis menyatakan, pengakuan itu akan memicu ketegangan dan krisis yang lebih besar lagi di Palestina. Melihat Resolusi PBB Nomor 2334 Tahun 2016, permukiman Israel di wilayah Palestina yang diduduki sejak tahun 1967 tidak memiliki keabsahan hukum. " Ini jelas tidak bisa diterima. Setiap langkah yang diambil AS, yang mengakui Yerusalem sebagai ibu kota Israel akan memicu ketegangan dan krisis lebih besar lagi di Palestina. Provokasi nyata bila itu terjadi, " kata Abdul Kharis melalui keterangan tertulis yang diterima kumparan (kumparan.com), Kamis (7 / 12). " Dalam resolusi di atas sudah jelas pemukiman saja kita tolak, ini kok malah memindahkan kedutaan, yang jelas ini melanggar resolusi dan menciderai nilai-nilai yang kita sepakati dalam forum internasional yang sah, saya minta Menlu untuk kirimkan nota protes kita ke Amerika Serikat dan PBB segera menggelar sidang darurat, " lanjut dia. Dalam Resolusi PBB Nomor 2334 Tahun 2016 juga menggarisbawahi tidak akan mengakui perubahan apapun dari garis-garis perbatasan 4 Juni 1967. Termasuk berkenaan dengan Yerusalem, selain yang disepakati oleh para pihak melalui negosiasi. " Merupakan pelanggaran mencolok di bawah hukum internasional dan merupakan kendala utama bagi pencapaian solusi dua negara dan perdamaian yang adil, abadi dan komprehensif, " ucap Abdul Kharis. Abdul Kharis juga memastikan bahwa langkah Amerika Serikat akan menyulitkan mereka dalam menjaga perdamaian di kawasan Timur Tengah khususnya Palestina. Bagi Palestina dengan mayoritas masyarakat muslim, langkah Trump tentu dianggap telah melampaui batas. " Apa yang sudah dan telah dilakukan selama ini dengan membawa Palestina dan Israel ke meja perundingan yang merupakan usaha Amerika Serikat menengahi konflik berkepanjangan antara kedua negara, yakni Palestina - Israel, akan semakin sulit terwujud, " tegasnya. Sebelumnya, Presiden Amerika Serikat, Donald Trump menyatakan inilah waktu yang tepat untuk memberikan pengakuan kepada Yerusalem sebagai ibu kota. " Saya telah menetapkan bahwa sekarang saatnya untuk secara resmi mengakui Yerusalem sebagai ibu kota Israel, " kata Trump di Gedung Putih seperti dikutip dari Associated Press (AP), Kamis (7 / 12). Trump juga telah memerintahkan kepada Kementerian Luar Negeri untuk memulai proses pemindahan kedutaan besar Amerika Serikat dari Tel Aviv ke Yerusalem. Proses ini diperkirakan akan memakan waktu hingga beberapa tahun.', 'Jakarta, CNN Indonesia - - Presiden Amerika Serikat Donald Trump dan Presiden Rusia Vladimir Putin berdiskusi mengenai solusi konflik Suriah hingga krisis nuklir Korea Utara melalui telepon pada Selasa (2 / 5) waktu setempat. Perbincangan kedua pemimpin ini merupakan yang pertama setelah hubungan Washington dan Moskow sempat merenggang akibat serangan udara AS ke Suriah, sekutu dekat Rusia, pada awal April lalu. Seorang pejabat senior AS \xa0 mengaku, Putin lah yang pertama kali meminta untuk menghubungi Trump. Dalam percakapan, Trump dan Putin dikabarkan sepakat meningkatkan dialog untuk mencari solusi memperkuat dan menjaga stabilitas gencatan senjata di Suriah. Keduanya juga turut membahas kemungkinan membentuk zona aman bagi warga sipil yang terdampak perang di negara Timur Tengah itu. Menurut Gedung Putih, kedua pemimpin sepakat bahwa " semua pihak wajib melakukan apa yang mereka bisa untuk mengakhiri kekerasan " di negara itu. " Percakapan mereka sangat baik, membahas zona aman atau de - eskalasi guna mencapai perdamaian kemanusiaan yang abadi dan berbagai persoalan lainnya, " bunyi pernyataan Gedung Putih pada Rabu (3 / 5). Kantor presiden AS itu menyebutkan, Trump juga menyatakan akan mengirimkan perwakilan negaranya sebagai pengamat \xa0 dalam perundingan gencatan senjata antara rezim Suriah dan kelompok oposisi di Astana, Kazakhstan pada Rabu dan Kamis pekan ini. Hal ini dinilai menggambarkan keseriusan AS untuk berkontribusi dalam upaya perdamaian Suriah. " Tujuannya untuk mendorong realisasi solusi damai bagi Suriah, " ucap kantor tersebut. Selain itu, Kremlin menyatakan, perbincangan Putin dan Trump turut membahas " solusi terbaik mengatasi situasi berbahaya di Korea Utara . " Korut terus menjadi sorotan setelah pada awal tahun baru lalu, pemimpin tertinggi mereka, Kim Jong - un, memerintahkan penguatan program rudal balistik antarbenua (ICBM) negaranya. Sepanjang tahun ini, Pyongyang tercatat sudah meluncurkan sejumlah uji coba rudal, dua di antaranya mencapai perairan di dekat wilayah Jepang. Dengan ambisi rudal nuklirnya, negara paling terisolasi ini menjadi salah satu tantangan utama global. Putin dan Trump turut mendiskusikan cara menyelesaikan krisis yang telah menimbulkan ketegangan di seluruh kawasan Asia Pasifik ini. " Situasi sangat berbahaya di Semenanjung Korea dibahas secara rinci. Presiden Putin menyerukan agar seluruh pihak menahan diri dan mengurangi ketegangan, " kata Kremlin seperti dilansir dari Reuters. Dalam kesempatan itu, kedua presiden juga turut mendiskusikan strategi memerangi terorisme dan kelompok militan di Timur Tengah, khususnya ISIS. Terorisme masih menjadi fokus utama keamanan bagi kedua negara. Putin dan Trump juga membahas rencana pertemuan tatap muka pertama mereka yang diagendakan berlangsung di sela-sela pertemuan KTT G - 20 do Hamburg pada 7 - 8 Juli mendatang.']</t>
         </is>
       </c>
     </row>
@@ -650,7 +650,7 @@
         <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>370</v>
+        <v>448</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -659,7 +659,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>['persen', 'indonesia', 'rp', 'pemerintah', 'harga', 'keuangan', 'industri', 'triliun', 'menteri', 'negara']</t>
+          <t>['persen', 'indonesia', 'rp', 'pemerintah', 'harga', 'games', 'negara', 'triliun', 'keuangan', 'menteri']</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -676,21 +676,21 @@
         <v>7</v>
       </c>
       <c r="C10" t="n">
-        <v>211</v>
+        <v>16</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>7_tubuh_kanker_kulit_penelitian</t>
+          <t>7_pasangan_hubungan_kado_orang</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>['tubuh', 'kanker', 'kulit', 'penelitian', 'tidur', 'orang', 'makan', 'makanan', 'kesehatan', 'penyakit']</t>
+          <t>['pasangan', 'hubungan', 'kado', 'orang', 'anak', 'bertengkar', 'cinta', 'pria', 'wanita', 'pernikahan']</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>['Buat sebagian orang, berolahraga dianggap cukup melelahkan, apalagi jika kamu juga berusaha untuk melakukan diet dan menurunkan berat badan. Namun, sadar atau enggak, untuk hidup sehat, kamu enggak perlu melakukan diet ketat atau olahraga berat setiap hari. Sebab, kamu cukup melakukan lima hal sederhana berikut ini, agar kamu mendapatkan tubuh yang sehat. Apa saja? Berikut rangkuman kumparan (kumparan.com) seperti yang dikutip dari Her World. 1. Buat makan siang sendiri Ini merupakan salah satu hal sederhana yang bisa kamu lakukan saat harus mengerjakan beberapa tugas menumpuk di kantor. Bangun lebih pagi dan memasukkan beberapa bahan makanan tertentu bisa membuat kamu lebih sehat. Hal ini juga bisa kamu lakukan saat makan malam. 2. Minum air yang cukup Minum air penting untuk menjaga cairan yang ada pada tubuh. Selain itu, meminum air yang cukup juga akan membantu kamu untuk mengurangi rasa lapar sehingga membuat kamu enggak mengonsumsi terlalu banyak makanan. Hal ini ampuh untuk menurunkan berat badan kamu, lho. 3. Jangan makan sampai kenyang Enggak semua makanan yang ada di atas piring makan siang kamu harus dilahap habis. Namun, hal ini bukan berarti kamu harus membuangnya, tapi kamu harus mengurangi porsi makanan sebelum menyantapnya. Otak membutuhkan waktu sekitar 20 menit untuk mendefinisikan bahwa tubuh kita sudah kenyang atau belum. Itu sebabnya, usahakan untuk mengendalikan jumlah makanan yang kamu makan. 4. Tidur yang cukup Ini merupakan salah satu cara paling mudah dan sempurna untuk kamu yang ingin hidup sehat. Tubuh membutuhkan waktu tidur sekitar 7 hingga 9 jam pada malam hari. Karenanya, singkirkan semua gangguan yang bisa mengganggu tidur kamu saat berada di tempat tidur ya. 5. Sayuran dan buah beku Sayur dan buah segar enggak bisa bertahan terlalu lama saat kamu membawanya pulang. Di sisi lain, kegiatan dan aktivitas kamu yang padat membuat kamu enggak bisa selalu belanja ke pasar atau supermarket untuk membeli sayur dan buah yang segar. Karenanya, coba ganti dengan sayur dan buah beku yang memiliki kandungan antioksidan dan nutrisi yang hampir sama dengan sayur dan buah yang segar.', 'Selain jantung dan stroke, kanker merupakan penyakit tidak menular yang paling ditakuti di dunia. Di Tanah Air sendiri, penyakit ini menduduki peringkat ketiga sebagai penyebab kematian. Pada 2012 lalu, kanker sedikitnya telah membunuh sekitar 8,2 juta manusia. Setahun kemudian, prevalensi penderita kanker meningkat jadi 1,4 persen. Kanker sendiri merupakan penyakit yang terjadi akibat mutasi sel tubuh menjadi sel kanker. Seiring berjalannya waktu, sel kanker ini akan menyebar ke seluruh tubuh. Jika terlambat ditangani, kanker bisa berakibat fatal dan mengakibatkan kematian. Penyakit ini disebabkan oleh banyak faktor. Mulai dari gaya hidup tak sehat (seperti merokok dan makanan mengandung bahan kimia), faktor keturunan, radikal bebas, stres, hingga infeksi virus. Penderita kanker biasanya akan mengalami perubahan fisik yang cukup drastis. Seperti perubahan warna kulit, wajah yang hampir selalu terlihat lelah, hingga berat badan yang merosot drastis. Perubahan bobot dan bentuk tubuh ini biasanya disebabkan oleh rasa nyeri pada tenggorokan dan mulutnya. Selain itu, penderita kanker juga akan sering merasa mual dan stres. Hal inilah yang menyebabkan hilangnya nafsu makan. Hilangnya nafsu makan tentunya akan berdampak pada asupan nutrisi yang diterima oleh penderita kanker. Padahal, nutrisi merupakan hal penting untuk membantu proses pemulihan pasien. Jika pasien mengalami kekurangan nutrisi atau malnutrisi, maka proses penyembuhan akan terhambat. " Malnutrisi memperlambat proses penyembuhan. Menyebabkan luka operasi susah sembuh, kemo dan radioterapi tidak maksimal, tumor tidak bisa mengecil, " jelas DR . Dr. Noorwat S. SpPD, KHOM saat ditemui kumparan (kumparan.com) di Hotel JS Luwansa, Jakarta Selatan, Selasa (29 / 8). aka " Malnutrisi bisa menyebabkan kaheksi, karena lemak dan ototnya hilang secara terus-menerus. Kaheksi bisa melelehkan lemak, membuat tidak nafsu makan, lambung penuh tidak mau makan. Akibatnya, sakit terus dan enggak sembuh - sembuh, " sambungnya lagi. Pada beberapa kasus yang parah, kaheksi bahkan membuat pasien kanker tinggal tulang berbalut kulit. Karena kekurangan nutrisi, pasien kanker jadi lemah dan tak bisa bergerak. Inilah mengapa banyak pasien akhirnya jadi tak berdaya dan meregang nyawa. Sayangnya, banyak orang yang belum menyadari dan masih menyepelekan pentingnya memperhatikan jumlah gizi yang masuk ke tubuh pasien kanker. Mitos seputar pantangan makan bagi orang kanker pun beredar luas. Seperti tak boleh makan daging, makanan bakaran, MSG, dan sebagainya. Padahal, larangan ini justru semakin mematahkan semangat hidup dan selera makan pasien kanker. Dukungan, energi positif, dan kesabaran keluarga sangat dibutuhkan untuk bisa melewati masa-masa ini. " Karena itu, penting untuk melihat nutrisi sebagai bagian dari pengobatan, " tutup Noorwati.', 'Jakarta, CNN Indonesia - - Kanker merupakan penyakit paling berisiko menyebabkan \xa0 kematian kedua di dunia. Di tahun 2015 angka kematian akibat kanker mencapai 8,8 juta. Ada beberapa kebiasaan yang bisa menyebabkan kanker. Misalnya kebiasaan buruk, berat badan, makanan yang kurang sehat, kurang aktivitas fisik, merokok dan konsumsi alkohol yang berlebih. Mengutip Boldsky, berikut kebiasaan buruk yang bisa menyebabkan kanker. 1. Pengharum ruangan Pengharum ruangan sering digunakan untuk mengatasi bau ruangan yang tidak sedap. Namun, pengharum ruangan ini tidak meningkatkan kualitas udara pada ruangan. Sebaliknya, pengharum ruangan mengandung zat berbahaya yang menyebabkan kanker. Zat berbahaya ini akan masuk ke hidung saat disemprotkan ke ruangan. 2. Minuman beralkohol Mengonsumsi minuman beralkohol telah terbukti dapat meningkatkan risiko kanker. Sebuah studi mencatat mengonsumsi minuman beralkohol dua kali dalam sehari dapat meningkatkan risiko kanker kerongkongan, kanker usus besar, kanker rektum dan kanker payudara. 3. Pil KB Pil KB, dikonsumsi untuk mencegah kehamilan. Mengonsumsi pil KB dapat meningkatkan risiko kanker payudara juga kanker serviks dan hati. 4. Lilin Sebuah penelitian mengatakan bahwa asap dari lilin parafin mengandung karsinogen dan komponen bahan bakar fosil lainnya. Untuk menggantikan penggunaan lilin parafin sebaiknya gunakan lilin lebah murni karena tidak berbahaya bagi tubuh. 5. Asap mobil Orang yang lebih sering terkena asap dari bahan bakar disel akan memiliki masalah kesehatan. Asap dari mobil bisa menyebabkan kanker paru-paru dan penyakit pernapasan lainnya. Diesel dan bensin melepaskan karbon monoksida dan hidrokarbon yang beracun. 6. Kosmetik Perempuan sering menggunakan make up untuk meningkatkan penampilan. Namun bahan kimia yang terkandung pada kosmetik akan tetap ada di dalam tubuh sekalipun sudah membersihkan wajah. Sebaiknya gunakan kosmetik dengan bahan organik untuk mengurangi risiko kanker kulit. 7. Makanan yang dibakar Ikan, ayam, atau makanan lain yang diolah dengan cara dibakar akan menyebabkan beberapa bagian menjadi gosong. Meskipun memiliki rasa yang lezat, makanan yang dibakar bisa meningkatkan risiko kanker perut, usus besar dan pankreas. 8. Makanan kaleng Wadah dari bahan logam yang digunakan untuk mengemas makanan mengandung bahan kimia berbahaya. Mengkonsumsi makanan kaleng akan menye babkan gangguan hormon dan perubahan DNA yang berakibat pada kanker payudara. 9. Diet Soda Diet soda mengandung pemanis buatan yang dapat meningkatkan kanker pankreas dan jenis kanker lainnya. Beberapa penelitian juga telah menunjukkan bahwa diet soda bisa menyebabkan kanker kandung kemih dan tumor otak.']</t>
+          <t>['Banyak orang yang berpendapat langgenggnya sebuah hubungan romansa ditentukan dari kesamaan hal yang disukai oleh kedua pasangan. Setujukah kamu dengan pendapat ini? Dilansir Metro, sebuah hubungan dikatakan akan berjalan harmonis dan bertahan lama jika kedua insan sama-sama menyukai hal yang sama. Bukan kesamaan jenis musik, jenis makanan, apalagi jenis buku yang dibaca, namun para peneliti mengatakan bahwa menyukai brand atau merek yang sama adalah kunci dari keberhasilan sebuah hubungan. Hmm...mungkin tak banyak dari kamu yang setuju dengan hasil penelitian ini. Namun ternyata berdasarkan penelitian dengan judul\' Coke vs Pepsi: Brand Compatibility, Relationship Power, and Life Satisfaction\' yang diterbitkan pada Journal of Consumer Research menunjukkan bahwa menyukai merek yang sama bisa berdampak pada kebahagiaan pasangan yang sedang menjalin kasih. Contohnya, jika kamu menyukai soda Coke dan pasangan kamu menyukai Pepsi maka perbedaan pendapat pun akan kamu temukan di sela-sela momen indah kalian. Perbedaan preferensi akan sebuah rasa dari kedua produk soda ini akan membuat kekuatan keseimbangan suatu hubungan menurun. " Jika kamu memiliki preferensi yang berbeda dengan pasangan, dan kamu adalah orang yang lemah dalam berargumen maka kamu akan merasa stuck dengan pandangan pasangan kamu akan suatu merek dan kamu harus dengan terpaksa menyetujui argumen pasangan kamu, " terang salah satu peneliti, Danielle Brick. " Semua pasangan tentu tak ingin merasakan perbedaan pendapat hanya karena sebuah merek saja, namun hal ini benar bisa memicu pertengkaran dan menyebabkan pasangan tak merasa bahagia, " sambungnya. Untuk mengetes teori ini, para peneliti melakukan sebuah tes sederhana dengan mengambil sampel dari beberapa merek termasuk produk minuman, cokelat, dan bahkan mobil. Dan hanya pasangan yang sudah menjalin hubungan lebih dari dua tahun yang boleh mengikuti tes ini. Para peneliti menganalisis tingkat kekuatan hubungan serta tingkat kebahagiaan para pasangan. Hasilnya menunjukkan perbedaan merek sebuah produk dapat menurunkan kadar bahagia seseorang. Periset juga melakukan beberapa penelitian terhadap preferensi merek dan sukacita sebuah hubungan, hasilnya pun tetap menunjukkan jawaban yang terus menerus sama. Meskipun perbedaan pendapat mengenai sebuah merek dapat memicu sebuah konflik, tapi Brick berujar perbedaan ini tak akan lantas membuat hubungan cepat berakhir. " Perbedaan agama dalam sebuah hubungan memang bisa menyebabkan kandasnya sebuah hubungan, namun perbedaan merek produk tak akan membuat hubungan yang sudah dijalani selama 11 tahun berakhir begitu saja, " papar Brick. Sejatinya, sebuah hubungan akan bertahan lama jika kedua pasangan bisa menerapkan sikap pengertian satu sama lain.', "Merdeka.com - Menjalani sebuah hubungan jangka panjang atau pernikahan, terkadang membuat seseorang tak lagi menghargai keberadaan pasangan seperti pada awal perkenalan. Ditambah dengan segudang aktivitas dan rutinitas yang membuat pasangan tidak lagi mementingkan kemesraan dan mengapresiasi satu sama lain dalam sebuah hubungan. Meski terlihat sepele, namun menunjukkan apresiasi atas hal-hal positif yang dilakukan pasangan adalah sesuatu yang penting untuk selalu dilakukan. Jika belum, coba lakukan cara-cara sederhana ini untuk membuat si dia merasa dihargai Jangan lupa untuk katakan terima kasih Hanya karena pasangan melakukan hal yang sama selama bertahun-tahun, bukan berarti ucapan terima kasih harus hilang, bukan? Sebab nyatanya Anda pun ingin pasangan menghargai segala yang sudah dilakukan. Oleh karena itu, untuk selanjutnya ketika pasangan sekadar menjemput Anda di kantor atau membawakan makanan kecil, jangan segan untuk mengatakan bahwa Anda sangat menghargai dan berterima kasih atas segala usaha yang dilakukan. Berikan sedikit ruang pribadi Setiap orang kadang perlu ruang untuk menyendiri, tak terkecuali pasangan Anda. Menjalani sebuah hubungan bukan berarti harus' menempel' terus tanpa memiliki ruang untuk diri sendiri. Jika pergi ke salon kecantikan tanpa anak-anak, bermain video game atau menonton pertandingan   sepak bola bisa membuat pasangan bahagia, berikan mereka waktu sesekali untuk melakukan hobinya atau sekadar bertemu dengan para sahabatnya. Jangan remehkan si dia, apalagi di depan orang lain Daripada merendahkan pasangan, lebih baik diskusikan segala masalah dengan si dia secara privat. Sebab mengeluh tentang masalah dengan pasangan di depan orang lain hanya akan membuat si dia sakit hati dan bersikap defensif, plus tanpa memberikan penyelesaian apapun. Jadi semarah apapun Anda dengan pasangan, biasakan untuk memiliki dialog dari hati ke hati dan temukanlah solusi terbaik dengan si dia. Lakukanlah hal kecil yang bermakna Actions speak louder than words. Jadi segala tindakan, bahkan yang sekecil apapun, mampu membuatnya merasa menjadi orang paling beruntung di dunia. Contoh, buatkan secangkir kopi ketika Anda tahu bahwa semalam pasangan harus kerja lembur, atau membuatkan semangkuk sup hangat dan obat ketika si dia sedang terserang flu. Lebih baik lagi jika bisa memberikan pasangan sedikit kejutan. Belikan hadiah yang Anda tahu pasangan pasti akan suka, misal buku favorit yang sudah lama dicari - cari atau mengajaknya ke restoran yang telah lama ingin ia kunjungi. Luangkan waktu bersama Meluangkan waktu untuk seseorang adalah sebuah hal yang sangat berharga, karena waktu adalah sesuatu yang tidak ternilai. Lagipula. siapa yang tidak ingin menghabiskan waktu berdua dengan orang dicintai? Rencanakan sebuah liburan romantis berdua, di mana Anda dan pasangan bisa menghabiskan waktu berkualitas bersama dan mengenang perjalanan bulan madu Anda dulu. Atau Anda juga bisa mendedikasikan satu hari dalam seminggu untuk kencan singkat yang romantis. [tsr]", 'Hubungan percintaan tak hanya didominasi kisah manis semata, ada kalanya beberapa hal bisa jadi \xa0 ancaman serius bagi hubungan \xa0 Anda dengan \xa0 pasangan. Itu sebabnya, sebelum memulai hubungan, pastikan Anda dan pasangan siap untuk saling menguatkan di kala suka maupun \xa0 duka. Karena jika tidak, bisa dipastikan hubungan Anda akan kandas di tengah jalan. Berikut adalah beberapa hal yang bisa bikin \xa0 hubungan Anda dan pasangan jadi kandas, seperti dilansir laman YourTango 1. Kepercayaan Kepercayaan sangat penting untuk mendapatkan hubungan yang langgeng. Tapi tak sedikit pasangan yang sulit menumbuhkan rasa percaya, karena traumatik pada hubungan sebelumnya. Belum lagi jika hubungan yang Anda jalani dipisahkan oleh jarak. Jika tak saling percaya, maka akan sulit untuk bertahan lama. 2. Selingkuh dan rasa cemburu Perselingkuhan merupakan noda dalam suatu hubungan. Akan sulit bagi pasangan lainnya menumbuhkan kepercayaan sepenuhnya. Meskipun Anda mengaku telah berubah, noda itu tak akan sepenuhnya hilang dari bayangan pasangan Anda. Bahkan tak jarang pasangan yang menjadi korban perselingkuhan akan memiliki rasa cemburu yang sangat besar. Jika sudah begini jarang ada hubungan yang bertahan lama. 3. Kesulitan berkomunikasi Komunikasi merupakan kunci untuk langgengnya suatu hubungan percintaan. Jika Anda dan pasangan memiliki hambatan dalam berkomunikasi maka hal ini akan menjadi ancaman bagi hubungan Anda. Apalagi perempuan merupakan golongan yang selalu ingin dimengerti dan dipahami, oleh karena itu komunikasi yang baik sangat dibutuhkan dalam suatu hubungan. 4. Pasangan terlalu dominan Hubungan asmara akan berjalan langgeng jika terjadi keseimbangan antar pasangan. Oleh karena itu sebaiknya hindari mendominasi suatu hubungan. Cobalah untuk saling memahami dan mendengarkan dalam suatu hubungan. Libatkan pasangan Anda dalam setiap keputusan bersama. 5. Kekerasan dalam hubungan Hubungan percintaan sejatinya ada untuk saling mengasihi. Oleh karena itu jika ada isu kekerasan dalam suatu hubungan, maka bisa dipastikan hubungan yang Anda jalani tak didasari oleh cinta. Adanya kekerasan dalam suatu hubungan pun merupakan ancaman bagi kelanggengan Anda dan pasangan. Sebelum memutuskan untuk bersama, ketahui lebih dulu siapa pasangan Anda.']</t>
         </is>
       </c>
     </row>
@@ -702,7 +702,7 @@
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['minyak', 'barel', 'mentah', 'opec', 'harga', 'produksi', 'persediaan', 'us', 'brent', 'juta']</t>
+          <t>['minyak', 'barel', 'mentah', 'opec', 'harga', 'produksi', 'persediaan', 'us', 'brent', 'dolar']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">

</xml_diff>